<commit_message>
Added new data and modified scripts in preparation for paleoclimate seminar
</commit_message>
<xml_diff>
--- a/Data/Boron/TJ_d11B_d18O_d13C.xlsx
+++ b/Data/Boron/TJ_d11B_d18O_d13C.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="424">
   <si>
     <t>sample</t>
   </si>
@@ -852,6 +852,261 @@
   </si>
   <si>
     <t>°C</t>
+  </si>
+  <si>
+    <t>LAV007</t>
+  </si>
+  <si>
+    <t>LAV003</t>
+  </si>
+  <si>
+    <t>LAV002</t>
+  </si>
+  <si>
+    <t>LAV012</t>
+  </si>
+  <si>
+    <t>LAV011</t>
+  </si>
+  <si>
+    <t>LAV010</t>
+  </si>
+  <si>
+    <t>LAV014</t>
+  </si>
+  <si>
+    <t>LAV016</t>
+  </si>
+  <si>
+    <t>LAV019</t>
+  </si>
+  <si>
+    <t>LAV020</t>
+  </si>
+  <si>
+    <t>LAV037</t>
+  </si>
+  <si>
+    <t>LAV021</t>
+  </si>
+  <si>
+    <t>LAV029</t>
+  </si>
+  <si>
+    <t>LAV030</t>
+  </si>
+  <si>
+    <t>LAV031</t>
+  </si>
+  <si>
+    <t>LAV038</t>
+  </si>
+  <si>
+    <t>LAV022</t>
+  </si>
+  <si>
+    <t>LAV025</t>
+  </si>
+  <si>
+    <t>LAV023</t>
+  </si>
+  <si>
+    <t>LAV039</t>
+  </si>
+  <si>
+    <t>LAV041</t>
+  </si>
+  <si>
+    <t>LAV040</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d11B</t>
+  </si>
+  <si>
+    <t>d11B_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>oneil_temperature</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature</t>
+  </si>
+  <si>
+    <t>hansen_temperature</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>hansen_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>delta_temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>LAV007</t>
+  </si>
+  <si>
+    <t>LAV003</t>
+  </si>
+  <si>
+    <t>LAV002</t>
+  </si>
+  <si>
+    <t>LAV012</t>
+  </si>
+  <si>
+    <t>LAV011</t>
+  </si>
+  <si>
+    <t>LAV010</t>
+  </si>
+  <si>
+    <t>LAV014</t>
+  </si>
+  <si>
+    <t>LAV016</t>
+  </si>
+  <si>
+    <t>LAV019</t>
+  </si>
+  <si>
+    <t>LAV020</t>
+  </si>
+  <si>
+    <t>LAV037</t>
+  </si>
+  <si>
+    <t>LAV021</t>
+  </si>
+  <si>
+    <t>LAV029</t>
+  </si>
+  <si>
+    <t>LAV030</t>
+  </si>
+  <si>
+    <t>LAV031</t>
+  </si>
+  <si>
+    <t>LAV038</t>
+  </si>
+  <si>
+    <t>LAV022</t>
+  </si>
+  <si>
+    <t>LAV025</t>
+  </si>
+  <si>
+    <t>LAV023</t>
+  </si>
+  <si>
+    <t>LAV039</t>
+  </si>
+  <si>
+    <t>LAV041</t>
+  </si>
+  <si>
+    <t>LAV040</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d11B</t>
+  </si>
+  <si>
+    <t>d11B_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>(2σ) ‰</t>
+  </si>
+  <si>
+    <t>‰ (pdb)</t>
+  </si>
+  <si>
+    <t>(1σ) ‰ (pdb)</t>
+  </si>
+  <si>
+    <t>‰ (pdb)</t>
+  </si>
+  <si>
+    <t>(1σ) ‰ (pdb)</t>
   </si>
   <si>
     <t>LAV007</t>
@@ -1083,7 +1338,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1118,11 +1373,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1145,6 +1408,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2163,696 +2434,703 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.19921875" customWidth="true"/>
-    <col min="2" max="2" width="5.6640625" customWidth="true"/>
-    <col min="3" max="4" width="11.6640625" customWidth="true"/>
-    <col min="5" max="5" width="13.6640625" customWidth="true"/>
-    <col min="6" max="6" width="6.265625" customWidth="true"/>
-    <col min="7" max="9" width="5.6640625" customWidth="true"/>
+    <col min="1" max="1" width="7.1796875" customWidth="true"/>
+    <col min="2" max="2" width="5.64453125" customWidth="true"/>
+    <col min="3" max="3" width="11.64453125" customWidth="true"/>
+    <col min="5" max="5" width="13.64453125" customWidth="true"/>
+    <col min="6" max="6" width="6.24609375" customWidth="true"/>
+    <col min="7" max="7" width="5.64453125" customWidth="true"/>
+    <col min="4" max="4" width="11.64453125" customWidth="true"/>
+    <col min="8" max="8" width="5.64453125" customWidth="true"/>
+    <col min="9" max="9" width="5.64453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>45</v>
+      <c r="A1" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
+      <c r="A2" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" s="0">
         <v>12.190000000000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>201.51597777778554</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>10.01219720849093</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>0.14363301630762756</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>-2.206</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>0.375</v>
       </c>
-      <c r="H3">
-        <v>-0.89</v>
-      </c>
-      <c r="I3">
+      <c r="H3" s="0">
+        <v>-0.89000000000000001</v>
+      </c>
+      <c r="I3" s="0">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B4" s="0">
         <v>13.59</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>201.47267350428129</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>10.24097362914215</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>0.11547829313839249</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>-0.72599999999999998</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>0.19</v>
       </c>
-      <c r="H4">
-        <v>2.4</v>
-      </c>
-      <c r="I4">
+      <c r="H4" s="0">
+        <v>2.3999999999999999</v>
+      </c>
+      <c r="I4" s="0">
         <v>0.81799999999999995</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B5" s="0">
         <v>14.59</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>201.45319851117404</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>9.9763254692479073</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>0.10441689371381085</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>-0.23100000000000001</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>0.432</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>3.7789999999999999</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>0.34699999999999998</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" s="0">
         <v>15.02</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>201.44486407500088</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>10.878138239162579</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>0.10350965730875188</v>
       </c>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
     </row>
     <row r="7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7">
-        <v>15.29</v>
-      </c>
-      <c r="C7">
+      <c r="A7" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B7" s="0">
+        <v>15.289999999999999</v>
+      </c>
+      <c r="C7" s="0">
         <v>201.4396940171018</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>9.8872299810538102</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>0.10382787734144472</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>-0.41399999999999998</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>0.32400000000000001</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>4.7679999999999998</v>
       </c>
-      <c r="I7">
-        <v>0.24</v>
+      <c r="I7" s="0">
+        <v>0.23999999999999999</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8">
-        <v>15.64</v>
-      </c>
-      <c r="C8">
+      <c r="A8" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B8" s="0">
+        <v>15.640000000000001</v>
+      </c>
+      <c r="C8" s="0">
         <v>201.43305299146076</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>10.708374995046363</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0.10475773652306104</v>
       </c>
-      <c r="F8">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="0">
+        <v>0.017999999999999999</v>
+      </c>
+      <c r="G8" s="0">
         <v>0.36299999999999999</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>3.9249999999999998</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>0.26400000000000001</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" s="0">
         <v>15.940000000000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>201.42736068376846</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>11.039549024903264</v>
       </c>
-      <c r="E9">
-        <v>9.7150894309145294E-2</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="0">
+        <v>0.097150894309145294</v>
+      </c>
+      <c r="F9" s="0">
         <v>-0.755</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>0.35499999999999998</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0">
         <v>3.8069999999999999</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>0.108</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B10" s="0">
         <v>16.190000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>201.42261709402487</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <v>10.762272249201416</v>
       </c>
-      <c r="E10">
-        <v>8.8684907140420544E-2</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="0">
+        <v>0.088684907140420544</v>
+      </c>
+      <c r="F10" s="0">
         <v>-0.97299999999999998</v>
       </c>
-      <c r="G10">
-        <v>0.26</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="0">
+        <v>0.26000000000000001</v>
+      </c>
+      <c r="H10" s="0">
         <v>3.5790000000000002</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="0">
         <v>0.249</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11">
-        <v>16.54</v>
-      </c>
-      <c r="C11">
+      <c r="A11" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B11" s="0">
+        <v>16.539999999999999</v>
+      </c>
+      <c r="C11" s="0">
         <v>201.41597606838383</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0">
         <v>10.835984879209818</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="0">
         <v>0.10998966327131669</v>
       </c>
-      <c r="F11">
-        <v>-0.51</v>
-      </c>
-      <c r="G11">
+      <c r="F11" s="0">
+        <v>-0.51000000000000001</v>
+      </c>
+      <c r="G11" s="0">
         <v>0.247</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>3.46</v>
       </c>
-      <c r="I11">
-        <v>8.4000000000000005E-2</v>
+      <c r="I11" s="0">
+        <v>0.084000000000000005</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12">
-        <v>16.89</v>
-      </c>
-      <c r="C12">
+      <c r="A12" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B12" s="0">
+        <v>16.890000000000001</v>
+      </c>
+      <c r="C12" s="0">
         <v>201.40933504274281</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="0">
         <v>10.459512485805641</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="0">
         <v>0.11454452430566182</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>-0.48199999999999998</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>0.17399999999999999</v>
       </c>
-      <c r="H12">
-        <v>2.69</v>
-      </c>
-      <c r="I12">
-        <v>7.1999999999999995E-2</v>
+      <c r="H12" s="0">
+        <v>2.6899999999999999</v>
+      </c>
+      <c r="I12" s="0">
+        <v>0.071999999999999995</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13">
-        <v>17.12</v>
-      </c>
-      <c r="C13">
+      <c r="A13" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B13" s="0">
+        <v>17.120000000000001</v>
+      </c>
+      <c r="C13" s="0">
         <v>201.40497094017871</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="0">
         <v>10.384159531398856</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="0">
         <v>0.11901469625718146</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>-0.59199999999999997</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>0.32900000000000001</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>2.6110000000000002</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" s="0">
         <v>17.490000000000002</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>201.39795042735821</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0">
         <v>9.9436806178566286</v>
       </c>
-      <c r="E14">
-        <v>9.6262499948600366E-2</v>
-      </c>
-      <c r="F14">
+      <c r="E14" s="0">
+        <v>0.096262499948600366</v>
+      </c>
+      <c r="F14" s="0">
         <v>-1.002</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>0.23100000000000001</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <v>2.6059999999999999</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <v>0.26600000000000001</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15">
-        <v>18.21</v>
-      </c>
-      <c r="C15">
+      <c r="A15" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B15" s="0">
+        <v>18.210000000000001</v>
+      </c>
+      <c r="C15" s="0">
         <v>201.38433722222999</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="0">
         <v>9.9960501404771449</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="0">
         <v>0.10589632985968327</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>-1.3320000000000001</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>0.81399999999999995</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <v>2.0099999999999998</v>
       </c>
-      <c r="I15">
-        <v>9.1999999999999998E-2</v>
+      <c r="I15" s="0">
+        <v>0.091999999999999998</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16">
+      <c r="A16" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B16" s="0">
         <v>18.439999999999998</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0">
         <v>201.38008222222999</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="0">
         <v>8.9507559822158029</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="0">
         <v>0.20756565956142378</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>-1.845</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>0.36699999999999999</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <v>1.248</v>
       </c>
-      <c r="I16">
-        <v>0.27</v>
+      <c r="I16" s="0">
+        <v>0.27000000000000002</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B17" s="0">
         <v>18.84</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="0">
         <v>201.37268222223</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="0">
         <v>9.2453681244467258</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="0">
         <v>0.1085995457562766</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>-0.68600000000000005</v>
       </c>
-      <c r="G17">
-        <v>3.9E-2</v>
-      </c>
-      <c r="H17">
+      <c r="G17" s="0">
+        <v>0.039</v>
+      </c>
+      <c r="H17" s="0">
         <v>2.8679999999999999</v>
       </c>
-      <c r="I17">
-        <v>5.8000000000000003E-2</v>
+      <c r="I17" s="0">
+        <v>0.058000000000000003</v>
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18">
-        <v>20.14</v>
-      </c>
-      <c r="C18">
+      <c r="A18" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B18" s="0">
+        <v>20.140000000000001</v>
+      </c>
+      <c r="C18" s="0">
         <v>201.34859722222998</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="0">
         <v>8.1044394762742993</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="0">
         <v>0.11800414700884421</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>-2.867</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>0.32100000000000001</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>1.5680000000000001</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <v>0.11</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19">
-        <v>20.64</v>
-      </c>
-      <c r="C19">
+      <c r="A19" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B19" s="0">
+        <v>20.640000000000001</v>
+      </c>
+      <c r="C19" s="0">
         <v>201.33922222223001</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="0">
         <v>9.7067607134899703</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="0">
         <v>0.10902200739197236</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>-1.587</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>0.161</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>1.758</v>
       </c>
-      <c r="I19">
-        <v>5.6000000000000001E-2</v>
+      <c r="I19" s="0">
+        <v>0.056000000000000001</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20">
-        <v>21.12</v>
-      </c>
-      <c r="C20">
+      <c r="A20" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B20" s="0">
+        <v>21.120000000000001</v>
+      </c>
+      <c r="C20" s="0">
         <v>201.33022222222999</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="0">
         <v>8.4942813608424057</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="0">
         <v>0.10853455716108885</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>-0.71299999999999997</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>0.33200000000000002</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>1.9830000000000001</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <v>0.20399999999999999</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21">
-        <v>21.14</v>
-      </c>
-      <c r="C21">
+      <c r="A21" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B21" s="0">
+        <v>21.140000000000001</v>
+      </c>
+      <c r="C21" s="0">
         <v>201.32984722223</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="0">
         <v>6.9697748282639225</v>
       </c>
-      <c r="E21">
-        <v>8.7536853144447743E-2</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="0">
+        <v>0.087536853144447743</v>
+      </c>
+      <c r="F21" s="0">
         <v>-1.5620000000000001</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0">
         <v>0.64500000000000002</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <v>1.726</v>
       </c>
-      <c r="I21">
-        <v>0.46</v>
+      <c r="I21" s="0">
+        <v>0.46000000000000002</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22">
-        <v>23.54</v>
-      </c>
-      <c r="C22">
+      <c r="A22" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B22" s="0">
+        <v>23.539999999999999</v>
+      </c>
+      <c r="C22" s="0">
         <v>201.28481196581973</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="0">
         <v>7.1065964233074652</v>
       </c>
-      <c r="E22">
-        <v>9.5202654485499486E-2</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="0">
+        <v>0.095202654485499486</v>
+      </c>
+      <c r="F22" s="0">
         <v>-1.0109999999999999</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0">
         <v>0.22900000000000001</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <v>2.056</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <v>0.12</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23">
-        <v>23.89</v>
-      </c>
-      <c r="C23">
+      <c r="A23" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B23" s="0">
+        <v>23.890000000000001</v>
+      </c>
+      <c r="C23" s="0">
         <v>201.27808119658897</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="0">
         <v>9.3714561608127696</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="0">
         <v>0.12036219998484181</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>-1.5880000000000001</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0">
         <v>0.14299999999999999</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <v>1.3129999999999999</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <v>0.246</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B24" s="0">
         <v>24.189999999999998</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="0">
         <v>201.27231196581974</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="0">
         <v>9.5039834385630684</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="0">
         <v>0.11997061322388737</v>
       </c>
-      <c r="F24">
-        <v>-0.9</v>
-      </c>
-      <c r="G24">
+      <c r="F24" s="0">
+        <v>-0.90000000000000002</v>
+      </c>
+      <c r="G24" s="0">
         <v>0.16600000000000001</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="0">
         <v>1.907</v>
       </c>
-      <c r="I24">
-        <v>3.7999999999999999E-2</v>
+      <c r="I24" s="0">
+        <v>0.037999999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2892,107 +3170,107 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.45">
       <c r="A1" s="0" t="s">
-        <v>294</v>
+        <v>379</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>295</v>
+        <v>380</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>296</v>
+        <v>381</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>297</v>
+        <v>382</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>298</v>
+        <v>383</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>300</v>
+        <v>385</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>301</v>
+        <v>386</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>302</v>
+        <v>387</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>303</v>
+        <v>388</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>304</v>
+        <v>389</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>305</v>
+        <v>390</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>306</v>
+        <v>391</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>307</v>
+        <v>392</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>308</v>
+        <v>393</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>309</v>
+        <v>394</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>311</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.45">
       <c r="A2" s="0" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>314</v>
+        <v>399</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>315</v>
+        <v>400</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>316</v>
+        <v>401</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>316</v>
+        <v>401</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>316</v>
+        <v>401</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>316</v>
+        <v>401</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>316</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.45">
       <c r="A3" s="0" t="s">
-        <v>317</v>
+        <v>402</v>
       </c>
       <c r="B3" s="0">
         <v>12.190000000000001</v>
@@ -3019,28 +3297,28 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="J3" s="0">
-        <v>28.368508465306718</v>
+        <v>28.352441634401487</v>
       </c>
       <c r="K3" s="0">
-        <v>29.324392362660205</v>
+        <v>29.30785541095247</v>
       </c>
       <c r="L3" s="0">
-        <v>29.833590643274853</v>
+        <v>29.820540540540541</v>
       </c>
       <c r="M3" s="0">
-        <v>30.869996506873221</v>
+        <v>30.853727076698316</v>
       </c>
       <c r="N3" s="0">
-        <v>3.7062098529601712</v>
+        <v>3.7056173370265242</v>
       </c>
       <c r="O3" s="0">
-        <v>3.8143457367965539</v>
+        <v>3.8139286534955659</v>
       </c>
       <c r="P3" s="0">
         <v>3</v>
       </c>
       <c r="Q3" s="0">
-        <v>3.7403875438596437</v>
+        <v>3.7397513513513481</v>
       </c>
       <c r="R3" s="0">
         <v>5.9254999999999995</v>
@@ -3048,7 +3326,7 @@
     </row>
     <row r="4" x14ac:dyDescent="0.45">
       <c r="A4" s="0" t="s">
-        <v>318</v>
+        <v>403</v>
       </c>
       <c r="B4" s="0">
         <v>13.59</v>
@@ -3075,36 +3353,36 @@
         <v>0.81799999999999995</v>
       </c>
       <c r="J4" s="0">
-        <v>21.316410887290999</v>
+        <v>21.301445182013083</v>
       </c>
       <c r="K4" s="0">
-        <v>21.985786501019447</v>
+        <v>21.970042230113506</v>
       </c>
       <c r="L4" s="0">
-        <v>23.913590643274855</v>
+        <v>23.90054054054054</v>
       </c>
       <c r="M4" s="0">
-        <v>23.773717086990182</v>
+        <v>23.758703076698318</v>
       </c>
       <c r="N4" s="0">
-        <v>1.7463906164867353</v>
+        <v>1.7461243509429778</v>
       </c>
       <c r="O4" s="0">
-        <v>1.8371785397287113</v>
+        <v>1.8369825312791477</v>
       </c>
       <c r="P4" s="0">
         <v>1.5199999999999996</v>
       </c>
       <c r="Q4" s="0">
-        <v>1.7489056888888861</v>
+        <v>1.7485833513513498</v>
       </c>
       <c r="R4" s="0">
-        <v>0.0055000000000013927</v>
+        <v>0.00549999999999784</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.45">
       <c r="A5" s="0" t="s">
-        <v>319</v>
+        <v>404</v>
       </c>
       <c r="B5" s="0">
         <v>14.59</v>
@@ -3131,28 +3409,28 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="J5" s="0">
-        <v>19.06813582300731</v>
+        <v>19.053510283317905</v>
       </c>
       <c r="K5" s="0">
-        <v>19.612476374814889</v>
+        <v>19.596984291686113</v>
       </c>
       <c r="L5" s="0">
-        <v>21.933590643274854</v>
+        <v>21.920540540540543</v>
       </c>
       <c r="M5" s="0">
-        <v>21.527390558042818</v>
+        <v>21.512796434806429</v>
       </c>
       <c r="N5" s="0">
-        <v>3.878916768283716</v>
+        <v>3.878334290039561</v>
       </c>
       <c r="O5" s="0">
-        <v>4.1083909475273117</v>
+        <v>4.1079561303309902</v>
       </c>
       <c r="P5" s="0">
-        <v>3.4560000000000031</v>
+        <v>3.4559999999999995</v>
       </c>
       <c r="Q5" s="0">
-        <v>3.8652624505263162</v>
+        <v>3.8645295567567572</v>
       </c>
       <c r="R5" s="0">
         <v>-1.974499999999999</v>
@@ -3160,7 +3438,7 @@
     </row>
     <row r="6" x14ac:dyDescent="0.45">
       <c r="A6" s="0" t="s">
-        <v>320</v>
+        <v>405</v>
       </c>
       <c r="B6" s="0">
         <v>15.02</v>
@@ -3190,7 +3468,7 @@
     </row>
     <row r="7" x14ac:dyDescent="0.45">
       <c r="A7" s="0" t="s">
-        <v>321</v>
+        <v>406</v>
       </c>
       <c r="B7" s="0">
         <v>15.289999999999999</v>
@@ -3217,28 +3495,28 @@
         <v>0.23999999999999999</v>
       </c>
       <c r="J7" s="0">
-        <v>19.893174061095181</v>
+        <v>19.878424297902825</v>
       </c>
       <c r="K7" s="0">
-        <v>20.485284875021648</v>
+        <v>20.469700284013811</v>
       </c>
       <c r="L7" s="0">
-        <v>22.665590643274854</v>
+        <v>22.652540540540542</v>
       </c>
       <c r="M7" s="0">
-        <v>22.350428188744569</v>
+        <v>22.335678834536157</v>
       </c>
       <c r="N7" s="0">
-        <v>2.9342906320148359</v>
+        <v>2.9338475410010574</v>
       </c>
       <c r="O7" s="0">
-        <v>3.1001900982059283</v>
+        <v>3.0998610144577015</v>
       </c>
       <c r="P7" s="0">
         <v>2.5919999999999987</v>
       </c>
       <c r="Q7" s="0">
-        <v>2.9297786778947383</v>
+        <v>2.9292290075675638</v>
       </c>
       <c r="R7" s="0">
         <v>-1.2424999999999997</v>
@@ -3246,7 +3524,7 @@
     </row>
     <row r="8" x14ac:dyDescent="0.45">
       <c r="A8" s="0" t="s">
-        <v>322</v>
+        <v>407</v>
       </c>
       <c r="B8" s="0">
         <v>15.640000000000001</v>
@@ -3273,28 +3551,28 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="J8" s="0">
-        <v>17.956891724449747</v>
+        <v>17.942432396368304</v>
       </c>
       <c r="K8" s="0">
-        <v>18.433437816290336</v>
+        <v>18.418070260754973</v>
       </c>
       <c r="L8" s="0">
-        <v>20.937590643274852</v>
+        <v>20.924540540540541</v>
       </c>
       <c r="M8" s="0">
-        <v>20.421503523481412</v>
+        <v>20.40712061615778</v>
       </c>
       <c r="N8" s="0">
-        <v>3.2214099831168141</v>
+        <v>3.2209299331026386</v>
       </c>
       <c r="O8" s="0">
-        <v>3.4235333171257594</v>
+        <v>3.4231724473782492</v>
       </c>
       <c r="P8" s="0">
-        <v>2.9039999999999999</v>
+        <v>2.9039999999999964</v>
       </c>
       <c r="Q8" s="0">
-        <v>3.2008929024561397</v>
+        <v>3.2002770681081074</v>
       </c>
       <c r="R8" s="0">
         <v>-2.9705000000000013</v>
@@ -3302,7 +3580,7 @@
     </row>
     <row r="9" x14ac:dyDescent="0.45">
       <c r="A9" s="0" t="s">
-        <v>323</v>
+        <v>408</v>
       </c>
       <c r="B9" s="0">
         <v>15.940000000000001</v>
@@ -3329,36 +3607,36 @@
         <v>0.108</v>
       </c>
       <c r="J9" s="0">
-        <v>21.449777505585416</v>
+        <v>21.434791457803613</v>
       </c>
       <c r="K9" s="0">
-        <v>22.126059460976478</v>
+        <v>22.110300220951274</v>
       </c>
       <c r="L9" s="0">
-        <v>24.029590643274855</v>
+        <v>24.016540540540539</v>
       </c>
       <c r="M9" s="0">
-        <v>23.907295535352759</v>
+        <v>23.892256925617239</v>
       </c>
       <c r="N9" s="0">
-        <v>3.2677097520627854</v>
+        <v>3.2672110482305357</v>
       </c>
       <c r="O9" s="0">
-        <v>3.4360746897518197</v>
+        <v>3.4357079118312868</v>
       </c>
       <c r="P9" s="0">
-        <v>2.8399999999999963</v>
+        <v>2.8399999999999999</v>
       </c>
       <c r="Q9" s="0">
-        <v>3.2730456081871324</v>
+        <v>3.2724433459459448</v>
       </c>
       <c r="R9" s="0">
-        <v>0.12150000000000105</v>
+        <v>0.1214999999999975</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.45">
       <c r="A10" s="0" t="s">
-        <v>324</v>
+        <v>409</v>
       </c>
       <c r="B10" s="0">
         <v>16.190000000000001</v>
@@ -3385,36 +3663,36 @@
         <v>0.249</v>
       </c>
       <c r="J10" s="0">
-        <v>22.458286915173744</v>
+        <v>22.443146441717374</v>
       </c>
       <c r="K10" s="0">
-        <v>23.184940388336372</v>
+        <v>23.169067921177884</v>
       </c>
       <c r="L10" s="0">
-        <v>24.901590643274854</v>
+        <v>24.888540540540539</v>
       </c>
       <c r="M10" s="0">
-        <v>24.918436954767962</v>
+        <v>24.903213425076697</v>
       </c>
       <c r="N10" s="0">
-        <v>2.4183545521154315</v>
+        <v>2.4179829599808045</v>
       </c>
       <c r="O10" s="0">
-        <v>2.5351544327439797</v>
+        <v>2.534882856019351</v>
       </c>
       <c r="P10" s="0">
         <v>2.0800000000000018</v>
       </c>
       <c r="Q10" s="0">
-        <v>2.4266337637426894</v>
+        <v>2.4261926702702716</v>
       </c>
       <c r="R10" s="0">
-        <v>0.99350000000000094</v>
+        <v>0.99349999999999739</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.45">
       <c r="A11" s="0" t="s">
-        <v>325</v>
+        <v>410</v>
       </c>
       <c r="B11" s="0">
         <v>16.539999999999999</v>
@@ -3441,28 +3719,28 @@
         <v>0.084000000000000005</v>
       </c>
       <c r="J11" s="0">
-        <v>20.328846006063657</v>
+        <v>20.314030362224571</v>
       </c>
       <c r="K11" s="0">
-        <v>20.945300295122593</v>
+        <v>20.929666836847957</v>
       </c>
       <c r="L11" s="0">
-        <v>23.049590643274854</v>
+        <v>23.036540540540543</v>
       </c>
       <c r="M11" s="0">
-        <v>22.785667554358604</v>
+        <v>22.770836767509127</v>
       </c>
       <c r="N11" s="0">
-        <v>2.2470907555500617</v>
+        <v>2.2467504372580152</v>
       </c>
       <c r="O11" s="0">
-        <v>2.3710259257108532</v>
+        <v>2.3707738511602656</v>
       </c>
       <c r="P11" s="0">
         <v>1.9759999999999991</v>
       </c>
       <c r="Q11" s="0">
-        <v>2.2458343555555516</v>
+        <v>2.2454153167567554</v>
       </c>
       <c r="R11" s="0">
         <v>-0.85849999999999937</v>
@@ -3470,7 +3748,7 @@
     </row>
     <row r="12" x14ac:dyDescent="0.45">
       <c r="A12" s="0" t="s">
-        <v>326</v>
+        <v>411</v>
       </c>
       <c r="B12" s="0">
         <v>16.890000000000001</v>
@@ -3497,28 +3775,28 @@
         <v>0.071999999999999995</v>
       </c>
       <c r="J12" s="0">
-        <v>20.201570015425091</v>
+        <v>20.186773638013847</v>
       </c>
       <c r="K12" s="0">
-        <v>20.810975743510426</v>
+        <v>20.795356562389486</v>
       </c>
       <c r="L12" s="0">
-        <v>22.937590643274852</v>
+        <v>22.924540540540541</v>
       </c>
       <c r="M12" s="0">
-        <v>22.658475219387846</v>
+        <v>22.643668183725346</v>
       </c>
       <c r="N12" s="0">
-        <v>1.5808375352659709</v>
+        <v>1.5805983335544624</v>
       </c>
       <c r="O12" s="0">
-        <v>1.6686906878657624</v>
+        <v>1.6685133642878895</v>
       </c>
       <c r="P12" s="0">
-        <v>1.3919999999999995</v>
+        <v>1.3919999999999959</v>
       </c>
       <c r="Q12" s="0">
-        <v>1.5795523003508762</v>
+        <v>1.5792571070270256</v>
       </c>
       <c r="R12" s="0">
         <v>-0.97050000000000125</v>
@@ -3526,7 +3804,7 @@
     </row>
     <row r="13" x14ac:dyDescent="0.45">
       <c r="A13" s="0" t="s">
-        <v>327</v>
+        <v>412</v>
       </c>
       <c r="B13" s="0">
         <v>17.120000000000001</v>
@@ -3553,36 +3831,36 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="J13" s="0">
-        <v>20.702558586265638</v>
+        <v>20.687686274983093</v>
       </c>
       <c r="K13" s="0">
-        <v>21.339408175135191</v>
+        <v>21.32373279008857</v>
       </c>
       <c r="L13" s="0">
-        <v>23.377590643274853</v>
+        <v>23.364540540540538</v>
       </c>
       <c r="M13" s="0">
-        <v>23.159331992487257</v>
+        <v>23.144431648590214</v>
       </c>
       <c r="N13" s="0">
-        <v>3.0048733097142986</v>
+        <v>3.0044170490835427</v>
       </c>
       <c r="O13" s="0">
-        <v>3.166940549263245</v>
+        <v>3.166603401854843</v>
       </c>
       <c r="P13" s="0">
-        <v>2.6319999999999979</v>
+        <v>2.6320000000000014</v>
       </c>
       <c r="Q13" s="0">
-        <v>3.005443551812867</v>
+        <v>3.004885398918919</v>
       </c>
       <c r="R13" s="0">
-        <v>-0.53049999999999997</v>
+        <v>-0.53050000000000352</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.45">
       <c r="A14" s="0" t="s">
-        <v>328</v>
+        <v>413</v>
       </c>
       <c r="B14" s="0">
         <v>17.490000000000002</v>
@@ -3609,36 +3887,36 @@
         <v>0.26600000000000001</v>
       </c>
       <c r="J14" s="0">
-        <v>22.593245151543385</v>
+        <v>22.578083932797654</v>
       </c>
       <c r="K14" s="0">
-        <v>23.326390792305972</v>
+        <v>23.310503169036622</v>
       </c>
       <c r="L14" s="0">
-        <v>25.017590643274854</v>
+        <v>25.004540540540539</v>
       </c>
       <c r="M14" s="0">
-        <v>25.053877783130535</v>
+        <v>25.038629653995617</v>
       </c>
       <c r="N14" s="0">
-        <v>2.1516020659128685</v>
+        <v>2.1512711636484028</v>
       </c>
       <c r="O14" s="0">
-        <v>2.2545942503088554</v>
+        <v>2.2543526140847803</v>
       </c>
       <c r="P14" s="0">
-        <v>1.847999999999999</v>
+        <v>1.8480000000000025</v>
       </c>
       <c r="Q14" s="0">
-        <v>2.1594542470175391</v>
+        <v>2.1590623524324357</v>
       </c>
       <c r="R14" s="0">
-        <v>1.1095000000000006</v>
+        <v>1.109499999999997</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.45">
       <c r="A15" s="0" t="s">
-        <v>329</v>
+        <v>414</v>
       </c>
       <c r="B15" s="0">
         <v>18.210000000000001</v>
@@ -3665,36 +3943,36 @@
         <v>0.091999999999999998</v>
       </c>
       <c r="J15" s="0">
-        <v>24.142392387593361</v>
+        <v>24.126991680942297</v>
       </c>
       <c r="K15" s="0">
-        <v>24.94585462401659</v>
+        <v>24.929792963240232</v>
       </c>
       <c r="L15" s="0">
-        <v>26.337590643274854</v>
+        <v>26.324540540540539</v>
       </c>
       <c r="M15" s="0">
-        <v>26.610502102428779</v>
+        <v>26.594974048590213</v>
       </c>
       <c r="N15" s="0">
-        <v>7.707244466978409</v>
+        <v>7.7060460653088967</v>
       </c>
       <c r="O15" s="0">
-        <v>8.0358722548998571</v>
+        <v>8.0350061567987154</v>
       </c>
       <c r="P15" s="0">
         <v>6.5120000000000005</v>
       </c>
       <c r="Q15" s="0">
-        <v>7.7491878418713434</v>
+        <v>7.7478068799999953</v>
       </c>
       <c r="R15" s="0">
-        <v>2.4295000000000009</v>
+        <v>2.4294999999999973</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.45">
       <c r="A16" s="0" t="s">
-        <v>330</v>
+        <v>415</v>
       </c>
       <c r="B16" s="0">
         <v>18.439999999999998</v>
@@ -3721,36 +3999,36 @@
         <v>0.27000000000000002</v>
       </c>
       <c r="J16" s="0">
-        <v>26.600751963797336</v>
+        <v>26.584966056638564</v>
       </c>
       <c r="K16" s="0">
-        <v>27.499901966408004</v>
+        <v>27.483563905581775</v>
       </c>
       <c r="L16" s="0">
-        <v>28.389590643274854</v>
+        <v>28.376540540540539</v>
       </c>
       <c r="M16" s="0">
-        <v>29.08656503242878</v>
+        <v>29.070601822914533</v>
       </c>
       <c r="N16" s="0">
-        <v>3.5624097083440347</v>
+        <v>3.5618468442275457</v>
       </c>
       <c r="O16" s="0">
-        <v>3.6867328633920806</v>
+        <v>3.6863321663659008</v>
       </c>
       <c r="P16" s="0">
-        <v>2.9359999999999999</v>
+        <v>2.9359999999999964</v>
       </c>
       <c r="Q16" s="0">
-        <v>3.5916993695906463</v>
+        <v>3.5910767491891846</v>
       </c>
       <c r="R16" s="0">
-        <v>4.4815000000000005</v>
+        <v>4.4814999999999969</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.45">
       <c r="A17" s="0" t="s">
-        <v>331</v>
+        <v>416</v>
       </c>
       <c r="B17" s="0">
         <v>18.84</v>
@@ -3777,28 +4055,28 @@
         <v>0.058000000000000003</v>
       </c>
       <c r="J17" s="0">
-        <v>21.132760123921287</v>
+        <v>21.117822400884393</v>
       </c>
       <c r="K17" s="0">
-        <v>21.79253177283158</v>
+        <v>21.776808113303218</v>
       </c>
       <c r="L17" s="0">
-        <v>23.753590643274855</v>
+        <v>23.740540540540543</v>
       </c>
       <c r="M17" s="0">
-        <v>23.589829751317669</v>
+        <v>23.574849671292917</v>
       </c>
       <c r="N17" s="0">
-        <v>0.35777721726469736</v>
+        <v>0.35772273790041709</v>
       </c>
       <c r="O17" s="0">
-        <v>0.37659258681514984</v>
+        <v>0.37655243486779</v>
       </c>
       <c r="P17" s="0">
-        <v>0.31199999999999761</v>
+        <v>0.31200000000000117</v>
       </c>
       <c r="Q17" s="0">
-        <v>0.35817470456140654</v>
+        <v>0.35810854054054175</v>
       </c>
       <c r="R17" s="0">
         <v>-0.15449999999999875</v>
@@ -3806,7 +4084,7 @@
     </row>
     <row r="18" x14ac:dyDescent="0.45">
       <c r="A18" s="0" t="s">
-        <v>332</v>
+        <v>417</v>
       </c>
       <c r="B18" s="0">
         <v>20.140000000000001</v>
@@ -3833,28 +4111,28 @@
         <v>0.11</v>
       </c>
       <c r="J18" s="0">
-        <v>31.689757920107127</v>
+        <v>31.673154316751209</v>
       </c>
       <c r="K18" s="0">
-        <v>32.724878633233061</v>
+        <v>32.707967777469037</v>
       </c>
       <c r="L18" s="0">
-        <v>32.477590643274851</v>
+        <v>32.46454054054054</v>
       </c>
       <c r="M18" s="0">
-        <v>34.223324458861526</v>
+        <v>34.206494331022647</v>
       </c>
       <c r="N18" s="0">
-        <v>3.2806092983597637</v>
+        <v>3.280073223415684</v>
       </c>
       <c r="O18" s="0">
-        <v>3.3410842788342734</v>
+        <v>3.3407148417139751</v>
       </c>
       <c r="P18" s="0">
         <v>2.5680000000000049</v>
       </c>
       <c r="Q18" s="0">
-        <v>3.3121058575438695</v>
+        <v>3.3115612767567626</v>
       </c>
       <c r="R18" s="0">
         <v>8.5694999999999979</v>
@@ -3862,7 +4140,7 @@
     </row>
     <row r="19" x14ac:dyDescent="0.45">
       <c r="A19" s="0" t="s">
-        <v>333</v>
+        <v>418</v>
       </c>
       <c r="B19" s="0">
         <v>20.640000000000001</v>
@@ -3889,28 +4167,28 @@
         <v>0.056000000000000001</v>
       </c>
       <c r="J19" s="0">
-        <v>25.356634931820736</v>
+        <v>25.341044758237672</v>
       </c>
       <c r="K19" s="0">
-        <v>26.209799268832796</v>
+        <v>26.193601118151435</v>
       </c>
       <c r="L19" s="0">
-        <v>27.357590643274854</v>
+        <v>27.344540540540542</v>
       </c>
       <c r="M19" s="0">
-        <v>27.832740917341063</v>
+        <v>27.81699655804967</v>
       </c>
       <c r="N19" s="0">
-        <v>1.5429089888784233</v>
+        <v>1.5426672504523822</v>
       </c>
       <c r="O19" s="0">
-        <v>1.6030240824543966</v>
+        <v>1.60285060882984</v>
       </c>
       <c r="P19" s="0">
-        <v>1.2879999999999967</v>
+        <v>1.2880000000000003</v>
       </c>
       <c r="Q19" s="0">
-        <v>1.55405037216374</v>
+        <v>1.5537772335135145</v>
       </c>
       <c r="R19" s="0">
         <v>3.4495000000000005</v>
@@ -3918,7 +4196,7 @@
     </row>
     <row r="20" x14ac:dyDescent="0.45">
       <c r="A20" s="0" t="s">
-        <v>334</v>
+        <v>419</v>
       </c>
       <c r="B20" s="0">
         <v>21.120000000000001</v>
@@ -3945,28 +4223,28 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="J20" s="0">
-        <v>21.256685873804656</v>
+        <v>21.241729272453995</v>
       </c>
       <c r="K20" s="0">
-        <v>21.922950092994199</v>
+        <v>21.907212525319437</v>
       </c>
       <c r="L20" s="0">
-        <v>23.861590643274852</v>
+        <v>23.84854054054054</v>
       </c>
       <c r="M20" s="0">
-        <v>23.713908072896615</v>
+        <v>23.698905089941562</v>
       </c>
       <c r="N20" s="0">
-        <v>3.049834565931576</v>
+        <v>3.0493697293505306</v>
       </c>
       <c r="O20" s="0">
-        <v>3.2088869670075155</v>
+        <v>3.2085446769575015</v>
       </c>
       <c r="P20" s="0">
         <v>2.6559999999999988</v>
       </c>
       <c r="Q20" s="0">
-        <v>3.0537382521637468</v>
+        <v>3.0531750097297277</v>
       </c>
       <c r="R20" s="0">
         <v>-0.046500000000001762</v>
@@ -3974,7 +4252,7 @@
     </row>
     <row r="21" x14ac:dyDescent="0.45">
       <c r="A21" s="0" t="s">
-        <v>335</v>
+        <v>420</v>
       </c>
       <c r="B21" s="0">
         <v>21.140000000000001</v>
@@ -4001,28 +4279,28 @@
         <v>0.46000000000000002</v>
       </c>
       <c r="J21" s="0">
-        <v>25.236919493006212</v>
+        <v>25.22134806813915</v>
       </c>
       <c r="K21" s="0">
-        <v>26.085395102299174</v>
+        <v>26.069210411302436</v>
       </c>
       <c r="L21" s="0">
-        <v>27.257590643274852</v>
+        <v>27.244540540540541</v>
       </c>
       <c r="M21" s="0">
-        <v>27.712166082545739</v>
+        <v>27.696442929671292</v>
       </c>
       <c r="N21" s="0">
-        <v>6.1752387470453982</v>
+        <v>6.174271675177863</v>
       </c>
       <c r="O21" s="0">
-        <v>6.4172900388056746</v>
+        <v>6.4165957937539133</v>
       </c>
       <c r="P21" s="0">
-        <v>5.1600000000000001</v>
+        <v>5.1599999999999966</v>
       </c>
       <c r="Q21" s="0">
-        <v>6.2174689754385994</v>
+        <v>6.2163747243243215</v>
       </c>
       <c r="R21" s="0">
         <v>3.349499999999999</v>
@@ -4030,7 +4308,7 @@
     </row>
     <row r="22" x14ac:dyDescent="0.45">
       <c r="A22" s="0" t="s">
-        <v>336</v>
+        <v>421</v>
       </c>
       <c r="B22" s="0">
         <v>23.539999999999999</v>
@@ -4057,28 +4335,28 @@
         <v>0.12</v>
       </c>
       <c r="J22" s="0">
-        <v>22.635167138259817</v>
+        <v>22.619999471564427</v>
       </c>
       <c r="K22" s="0">
-        <v>23.37031749031928</v>
+        <v>23.354425158926517</v>
       </c>
       <c r="L22" s="0">
-        <v>25.053590643274852</v>
+        <v>25.04054054054054</v>
       </c>
       <c r="M22" s="0">
-        <v>25.095955603656851</v>
+        <v>25.080699840211832</v>
       </c>
       <c r="N22" s="0">
-        <v>2.1338986620505693</v>
+        <v>2.1335703896642713</v>
       </c>
       <c r="O22" s="0">
-        <v>2.2357558717813504</v>
+        <v>2.2355162191215072</v>
       </c>
       <c r="P22" s="0">
         <v>1.8320000000000007</v>
       </c>
       <c r="Q22" s="0">
-        <v>2.1418293934502977</v>
+        <v>2.1414408918918895</v>
       </c>
       <c r="R22" s="0">
         <v>1.1454999999999984</v>
@@ -4086,7 +4364,7 @@
     </row>
     <row r="23" x14ac:dyDescent="0.45">
       <c r="A23" s="0" t="s">
-        <v>337</v>
+        <v>422</v>
       </c>
       <c r="B23" s="0">
         <v>23.890000000000001</v>
@@ -4113,36 +4391,36 @@
         <v>0.246</v>
       </c>
       <c r="J23" s="0">
-        <v>25.361426609373666</v>
+        <v>25.345835685050019</v>
       </c>
       <c r="K23" s="0">
-        <v>26.214777651896839</v>
+        <v>26.198578962472311</v>
       </c>
       <c r="L23" s="0">
-        <v>27.361590643274855</v>
+        <v>27.34854054054054</v>
       </c>
       <c r="M23" s="0">
-        <v>27.837567290732874</v>
+        <v>27.821822083184806</v>
       </c>
       <c r="N23" s="0">
-        <v>1.3704722022345095</v>
+        <v>1.3702574748288612</v>
       </c>
       <c r="O23" s="0">
-        <v>1.4238504944194119</v>
+        <v>1.4236964080063217</v>
       </c>
       <c r="P23" s="0">
-        <v>1.1439999999999984</v>
+        <v>1.1440000000000019</v>
       </c>
       <c r="Q23" s="0">
-        <v>1.380379970058474</v>
+        <v>1.3801373686486542</v>
       </c>
       <c r="R23" s="0">
-        <v>3.4535000000000018</v>
+        <v>3.4534999999999982</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.45">
       <c r="A24" s="0" t="s">
-        <v>338</v>
+        <v>423</v>
       </c>
       <c r="B24" s="0">
         <v>24.189999999999998</v>
@@ -4169,31 +4447,31 @@
         <v>0.037999999999999999</v>
       </c>
       <c r="J24" s="0">
-        <v>22.119397945882099</v>
+        <v>22.104309481771111</v>
       </c>
       <c r="K24" s="0">
-        <v>22.829490495742505</v>
+        <v>22.81365608236473</v>
       </c>
       <c r="L24" s="0">
-        <v>24.609590643274856</v>
+        <v>24.596540540540541</v>
       </c>
       <c r="M24" s="0">
-        <v>24.578467677165623</v>
+        <v>24.563306070211834</v>
       </c>
       <c r="N24" s="0">
-        <v>1.5385700281526624</v>
+        <v>1.5383341688890368</v>
       </c>
       <c r="O24" s="0">
-        <v>1.6145813543581653</v>
+        <v>1.6144086027890125</v>
       </c>
       <c r="P24" s="0">
         <v>1.3279999999999994</v>
       </c>
       <c r="Q24" s="0">
-        <v>1.5430109660818729</v>
+        <v>1.5427293448648634</v>
       </c>
       <c r="R24" s="0">
-        <v>0.7015000000000029</v>
+        <v>0.70149999999999935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big update to change data files, adding additional criteria for point rejection, and trialling additional smoothing of the ensemble.
</commit_message>
<xml_diff>
--- a/Data/Boron/TJ_d11B_d18O_d13C.xlsx
+++ b/Data/Boron/TJ_d11B_d18O_d13C.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross\Documents\Work\Postdoc\St_Andrews\Repositories\Triassic-Jurassic-CO2\Data\Boron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Work\Postdoc\St_Andrews\Repositories\Triassic-Jurassic-CO2\Data\Boron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8CCD1F-FBFA-4D83-807A-B1F2400424FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC7F4CF-D280-424E-96BB-C66EF4EAFA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2"/>
+    <workbookView xWindow="4417" yWindow="2258" windowWidth="12128" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="With_Age" sheetId="5" r:id="rId2"/>
-    <sheet name="Temperature_Calibrations" sheetId="6" r:id="rId3"/>
+    <sheet name="With_Age" sheetId="2" r:id="rId2"/>
+    <sheet name="Temperature_Calibrations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="220">
   <si>
     <t>sample</t>
   </si>
@@ -137,18 +137,420 @@
     <t>d13C_uncertainty</t>
   </si>
   <si>
+    <t>‰ (pdb)</t>
+  </si>
+  <si>
+    <t>(1σ) ‰ (pdb)</t>
+  </si>
+  <si>
+    <t>number_of_replicates</t>
+  </si>
+  <si>
+    <t>diagenetic_alteration</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d11B</t>
+  </si>
+  <si>
+    <t>d11B_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>number_of_replicates</t>
+  </si>
+  <si>
+    <t>diagenetic_alteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>(2σ) ‰</t>
+  </si>
+  <si>
+    <t>‰ (pdb)</t>
+  </si>
+  <si>
+    <t>(1σ) ‰ (pdb)</t>
+  </si>
+  <si>
+    <t>‰ (pdb)</t>
+  </si>
+  <si>
+    <t>(1σ) ‰ (pdb)</t>
+  </si>
+  <si>
+    <t>LAV007</t>
+  </si>
+  <si>
+    <t>LAV003</t>
+  </si>
+  <si>
+    <t>LAV002</t>
+  </si>
+  <si>
+    <t>LAV012</t>
+  </si>
+  <si>
+    <t>LAV011</t>
+  </si>
+  <si>
+    <t>LAV010</t>
+  </si>
+  <si>
+    <t>LAV014</t>
+  </si>
+  <si>
+    <t>LAV016</t>
+  </si>
+  <si>
+    <t>LAV019</t>
+  </si>
+  <si>
+    <t>LAV020</t>
+  </si>
+  <si>
+    <t>LAV037</t>
+  </si>
+  <si>
+    <t>LAV021</t>
+  </si>
+  <si>
+    <t>LAV029</t>
+  </si>
+  <si>
+    <t>LAV030</t>
+  </si>
+  <si>
+    <t>LAV031</t>
+  </si>
+  <si>
+    <t>LAV038</t>
+  </si>
+  <si>
+    <t>LAV022</t>
+  </si>
+  <si>
+    <t>LAV025</t>
+  </si>
+  <si>
+    <t>LAV023</t>
+  </si>
+  <si>
+    <t>LAV039</t>
+  </si>
+  <si>
+    <t>LAV041</t>
+  </si>
+  <si>
+    <t>LAV040</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d11B</t>
+  </si>
+  <si>
+    <t>d11B_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>number_of_replicates</t>
+  </si>
+  <si>
+    <t>diagenetic_alteration</t>
+  </si>
+  <si>
+    <t>oneil_temperature</t>
+  </si>
+  <si>
+    <t>oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>hansen_temperature</t>
+  </si>
+  <si>
+    <t>hansen_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>delta_temperature</t>
+  </si>
+  <si>
+    <t>delta_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
     <t>°C</t>
   </si>
   <si>
+    <t>LAV007</t>
+  </si>
+  <si>
+    <t>LAV003</t>
+  </si>
+  <si>
+    <t>LAV002</t>
+  </si>
+  <si>
+    <t>LAV012</t>
+  </si>
+  <si>
+    <t>LAV011</t>
+  </si>
+  <si>
+    <t>LAV010</t>
+  </si>
+  <si>
+    <t>LAV014</t>
+  </si>
+  <si>
+    <t>LAV016</t>
+  </si>
+  <si>
+    <t>LAV019</t>
+  </si>
+  <si>
+    <t>LAV020</t>
+  </si>
+  <si>
+    <t>LAV037</t>
+  </si>
+  <si>
+    <t>LAV021</t>
+  </si>
+  <si>
+    <t>LAV029</t>
+  </si>
+  <si>
+    <t>LAV030</t>
+  </si>
+  <si>
+    <t>LAV031</t>
+  </si>
+  <si>
+    <t>LAV038</t>
+  </si>
+  <si>
+    <t>LAV022</t>
+  </si>
+  <si>
+    <t>LAV025</t>
+  </si>
+  <si>
+    <t>LAV023</t>
+  </si>
+  <si>
+    <t>LAV039</t>
+  </si>
+  <si>
+    <t>LAV041</t>
+  </si>
+  <si>
+    <t>LAV040</t>
+  </si>
+  <si>
+    <t>al_ca_reject</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d11B</t>
+  </si>
+  <si>
+    <t>d11B_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>number_of_replicates</t>
+  </si>
+  <si>
+    <t>diagenetic_alteration</t>
+  </si>
+  <si>
+    <t>al_ca_reject</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>(2σ) ‰</t>
+  </si>
+  <si>
     <t>‰ (pdb)</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>(1σ) ‰ (pdb)</t>
   </si>
   <si>
+    <t>‰ (pdb)</t>
+  </si>
+  <si>
+    <t>(1σ) ‰ (pdb)</t>
+  </si>
+  <si>
+    <t>LAV007</t>
+  </si>
+  <si>
+    <t>LAV003</t>
+  </si>
+  <si>
+    <t>LAV002</t>
+  </si>
+  <si>
+    <t>LAV012</t>
+  </si>
+  <si>
+    <t>LAV011</t>
+  </si>
+  <si>
+    <t>LAV010</t>
+  </si>
+  <si>
+    <t>LAV014</t>
+  </si>
+  <si>
+    <t>LAV016</t>
+  </si>
+  <si>
+    <t>LAV019</t>
+  </si>
+  <si>
+    <t>LAV020</t>
+  </si>
+  <si>
+    <t>LAV037</t>
+  </si>
+  <si>
+    <t>LAV021</t>
+  </si>
+  <si>
+    <t>LAV029</t>
+  </si>
+  <si>
+    <t>LAV030</t>
+  </si>
+  <si>
+    <t>LAV031</t>
+  </si>
+  <si>
+    <t>LAV038</t>
+  </si>
+  <si>
+    <t>LAV022</t>
+  </si>
+  <si>
+    <t>LAV025</t>
+  </si>
+  <si>
+    <t>LAV023</t>
+  </si>
+  <si>
+    <t>LAV039</t>
+  </si>
+  <si>
+    <t>LAV041</t>
+  </si>
+  <si>
+    <t>LAV040</t>
+  </si>
+  <si>
     <t>sample</t>
   </si>
   <si>
@@ -176,1057 +578,43 @@
     <t>d13C_uncertainty</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>(2σ) ‰</t>
-  </si>
-  <si>
-    <t>‰ (pdb)</t>
-  </si>
-  <si>
-    <t>(1σ) ‰ (pdb)</t>
-  </si>
-  <si>
-    <t>‰ (pdb)</t>
-  </si>
-  <si>
-    <t>(1σ) ‰ (pdb)</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
+    <t>number_of_replicates</t>
+  </si>
+  <si>
+    <t>diagenetic_alteration</t>
+  </si>
+  <si>
+    <t>al_ca_reject</t>
   </si>
   <si>
     <t>oneil_temperature</t>
   </si>
   <si>
+    <t>oneil_temperature_uncertainty</t>
+  </si>
+  <si>
     <t>kim_oneil_temperature</t>
   </si>
   <si>
+    <t>kim_oneil_temperature_uncertainty</t>
+  </si>
+  <si>
     <t>hansen_temperature</t>
   </si>
   <si>
+    <t>hansen_temperature_uncertainty</t>
+  </si>
+  <si>
     <t>anderson_arthur_temperature</t>
   </si>
   <si>
+    <t>anderson_arthur_temperature_uncertainty</t>
+  </si>
+  <si>
     <t>delta_temperature</t>
   </si>
   <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>oneil_temperature</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature</t>
-  </si>
-  <si>
-    <t>hansen_temperature</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>oneil_temperature</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature</t>
-  </si>
-  <si>
-    <t>hansen_temperature</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature</t>
-  </si>
-  <si>
-    <t>oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>hansen_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>oneil_temperature</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature</t>
-  </si>
-  <si>
-    <t>hansen_temperature</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature</t>
-  </si>
-  <si>
-    <t>oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>hansen_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>oneil_temperature</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature</t>
-  </si>
-  <si>
-    <t>hansen_temperature</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature</t>
-  </si>
-  <si>
-    <t>oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>hansen_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>oneil_temperature</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature</t>
-  </si>
-  <si>
-    <t>hansen_temperature</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature</t>
-  </si>
-  <si>
-    <t>oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>hansen_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>(2σ) ‰</t>
-  </si>
-  <si>
-    <t>‰ (pdb)</t>
-  </si>
-  <si>
-    <t>(1σ) ‰ (pdb)</t>
-  </si>
-  <si>
-    <t>‰ (pdb)</t>
-  </si>
-  <si>
-    <t>(1σ) ‰ (pdb)</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>oneil_temperature</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature</t>
-  </si>
-  <si>
-    <t>hansen_temperature</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature</t>
-  </si>
-  <si>
-    <t>oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>kim_oneil_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>hansen_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>anderson_arthur_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
+    <t>delta_temperature_uncertainty</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -1314,7 +702,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1329,6 +720,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1338,7 +736,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="11">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -1361,34 +766,17 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="true"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
@@ -1397,28 +785,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{A13D6E8E-3877-43C7-98E4-DD8D2AF0492C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1730,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68F4B3C-2083-4337-8469-4076B988F653}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="true" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1771,6 +1141,12 @@
       <c r="I1" t="s">
         <v>35</v>
       </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
@@ -1783,16 +1159,16 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
       <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
         <v>34</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.45">
@@ -1823,6 +1199,12 @@
       <c r="I3" s="1">
         <v>10</v>
       </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -1852,6 +1234,12 @@
       <c r="I4" s="1">
         <v>10</v>
       </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -1881,19 +1269,46 @@
       <c r="I5" s="1">
         <v>6</v>
       </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>15.02</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>10.878138239162579</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.10350965730875188</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-0.15657041491121942</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.15658315377321824</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.4725361218805384</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.10379699156144404</v>
+      </c>
+      <c r="I6" s="3">
+        <v>12</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.45">
@@ -1924,6 +1339,12 @@
       <c r="I7" s="1">
         <v>15</v>
       </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -1953,6 +1374,12 @@
       <c r="I8" s="1">
         <v>6</v>
       </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -1982,6 +1409,12 @@
       <c r="I9" s="1">
         <v>6</v>
       </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -2011,6 +1444,12 @@
       <c r="I10" s="1">
         <v>5</v>
       </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -2040,6 +1479,12 @@
       <c r="I11" s="1">
         <v>6</v>
       </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -2069,6 +1514,12 @@
       <c r="I12" s="1">
         <v>6</v>
       </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -2098,6 +1549,12 @@
       <c r="I13" s="1">
         <v>10</v>
       </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -2127,6 +1584,12 @@
       <c r="I14" s="1">
         <v>18</v>
       </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
@@ -2156,6 +1619,12 @@
       <c r="I15" s="1">
         <v>6</v>
       </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -2185,6 +1654,12 @@
       <c r="I16" s="1">
         <v>18</v>
       </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
@@ -2214,6 +1689,12 @@
       <c r="I17" s="1">
         <v>8</v>
       </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
@@ -2243,6 +1724,12 @@
       <c r="I18" s="1">
         <v>7</v>
       </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
@@ -2272,6 +1759,12 @@
       <c r="I19" s="1">
         <v>8</v>
       </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
@@ -2301,6 +1794,12 @@
       <c r="I20" s="1">
         <v>7</v>
       </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
@@ -2330,6 +1829,12 @@
       <c r="I21" s="1">
         <v>22</v>
       </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
@@ -2359,6 +1864,12 @@
       <c r="I22" s="1">
         <v>6</v>
       </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
@@ -2388,6 +1899,12 @@
       <c r="I23" s="1">
         <v>6</v>
       </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
@@ -2416,6 +1933,12 @@
       </c>
       <c r="I24" s="1">
         <v>9</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2425,12 +1948,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2438,74 +1959,86 @@
     <col min="2" max="2" width="5.64453125" customWidth="true"/>
     <col min="3" max="3" width="11.64453125" customWidth="true"/>
     <col min="5" max="5" width="13.64453125" customWidth="true"/>
-    <col min="6" max="6" width="6.24609375" customWidth="true"/>
-    <col min="7" max="7" width="5.64453125" customWidth="true"/>
+    <col min="6" max="6" width="13.24609375" customWidth="true"/>
+    <col min="7" max="7" width="12.64453125" customWidth="true"/>
+    <col min="8" max="8" width="11.64453125" customWidth="true"/>
+    <col min="9" max="9" width="12.64453125" customWidth="true"/>
+    <col min="10" max="10" width="3.1796875" customWidth="true"/>
+    <col min="11" max="11" width="2.1796875" customWidth="true"/>
     <col min="4" max="4" width="11.64453125" customWidth="true"/>
-    <col min="8" max="8" width="5.64453125" customWidth="true"/>
-    <col min="9" max="9" width="5.64453125" customWidth="true"/>
+    <col min="12" max="12" width="2.1796875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.45">
       <c r="A1" s="0" t="s">
-        <v>339</v>
+        <v>128</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>340</v>
+        <v>129</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>341</v>
+        <v>130</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>342</v>
+        <v>131</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>343</v>
+        <v>132</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>344</v>
+        <v>133</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>345</v>
+        <v>134</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>346</v>
+        <v>135</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>347</v>
+        <v>136</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.45">
       <c r="A2" s="0" t="s">
-        <v>348</v>
+        <v>140</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>349</v>
+        <v>141</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>350</v>
+        <v>142</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>351</v>
+        <v>143</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>352</v>
+        <v>144</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>353</v>
+        <v>145</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>354</v>
+        <v>146</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>355</v>
+        <v>147</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>356</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.45">
       <c r="A3" s="0" t="s">
-        <v>357</v>
+        <v>149</v>
       </c>
       <c r="B3" s="0">
         <v>12.190000000000001</v>
@@ -2531,10 +2064,19 @@
       <c r="I3" s="0">
         <v>0.56999999999999995</v>
       </c>
+      <c r="J3" s="0">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0">
+        <v>1</v>
+      </c>
+      <c r="L3" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" x14ac:dyDescent="0.45">
       <c r="A4" s="0" t="s">
-        <v>358</v>
+        <v>150</v>
       </c>
       <c r="B4" s="0">
         <v>13.59</v>
@@ -2560,10 +2102,19 @@
       <c r="I4" s="0">
         <v>0.81799999999999995</v>
       </c>
+      <c r="J4" s="0">
+        <v>10</v>
+      </c>
+      <c r="K4" s="0">
+        <v>0</v>
+      </c>
+      <c r="L4" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" x14ac:dyDescent="0.45">
       <c r="A5" s="0" t="s">
-        <v>359</v>
+        <v>151</v>
       </c>
       <c r="B5" s="0">
         <v>14.59</v>
@@ -2589,10 +2140,19 @@
       <c r="I5" s="0">
         <v>0.34699999999999998</v>
       </c>
+      <c r="J5" s="0">
+        <v>6</v>
+      </c>
+      <c r="K5" s="0">
+        <v>0</v>
+      </c>
+      <c r="L5" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" x14ac:dyDescent="0.45">
       <c r="A6" s="0" t="s">
-        <v>360</v>
+        <v>152</v>
       </c>
       <c r="B6" s="0">
         <v>15.02</v>
@@ -2606,14 +2166,31 @@
       <c r="E6" s="0">
         <v>0.10350965730875188</v>
       </c>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
+      <c r="F6" s="0">
+        <v>-0.15657041491121942</v>
+      </c>
+      <c r="G6" s="0">
+        <v>0.15658315377321824</v>
+      </c>
+      <c r="H6" s="0">
+        <v>4.4725361218805384</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0.10379699156144404</v>
+      </c>
+      <c r="J6" s="0">
+        <v>12</v>
+      </c>
+      <c r="K6" s="0">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" x14ac:dyDescent="0.45">
       <c r="A7" s="0" t="s">
-        <v>361</v>
+        <v>153</v>
       </c>
       <c r="B7" s="0">
         <v>15.289999999999999</v>
@@ -2639,10 +2216,19 @@
       <c r="I7" s="0">
         <v>0.23999999999999999</v>
       </c>
+      <c r="J7" s="0">
+        <v>15</v>
+      </c>
+      <c r="K7" s="0">
+        <v>0</v>
+      </c>
+      <c r="L7" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" x14ac:dyDescent="0.45">
       <c r="A8" s="0" t="s">
-        <v>362</v>
+        <v>154</v>
       </c>
       <c r="B8" s="0">
         <v>15.640000000000001</v>
@@ -2668,10 +2254,19 @@
       <c r="I8" s="0">
         <v>0.26400000000000001</v>
       </c>
+      <c r="J8" s="0">
+        <v>6</v>
+      </c>
+      <c r="K8" s="0">
+        <v>0</v>
+      </c>
+      <c r="L8" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" x14ac:dyDescent="0.45">
       <c r="A9" s="0" t="s">
-        <v>363</v>
+        <v>155</v>
       </c>
       <c r="B9" s="0">
         <v>15.940000000000001</v>
@@ -2697,10 +2292,19 @@
       <c r="I9" s="0">
         <v>0.108</v>
       </c>
+      <c r="J9" s="0">
+        <v>6</v>
+      </c>
+      <c r="K9" s="0">
+        <v>0</v>
+      </c>
+      <c r="L9" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" x14ac:dyDescent="0.45">
       <c r="A10" s="0" t="s">
-        <v>364</v>
+        <v>156</v>
       </c>
       <c r="B10" s="0">
         <v>16.190000000000001</v>
@@ -2726,10 +2330,19 @@
       <c r="I10" s="0">
         <v>0.249</v>
       </c>
+      <c r="J10" s="0">
+        <v>5</v>
+      </c>
+      <c r="K10" s="0">
+        <v>0</v>
+      </c>
+      <c r="L10" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" x14ac:dyDescent="0.45">
       <c r="A11" s="0" t="s">
-        <v>365</v>
+        <v>157</v>
       </c>
       <c r="B11" s="0">
         <v>16.539999999999999</v>
@@ -2755,10 +2368,19 @@
       <c r="I11" s="0">
         <v>0.084000000000000005</v>
       </c>
+      <c r="J11" s="0">
+        <v>6</v>
+      </c>
+      <c r="K11" s="0">
+        <v>0</v>
+      </c>
+      <c r="L11" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" x14ac:dyDescent="0.45">
       <c r="A12" s="0" t="s">
-        <v>366</v>
+        <v>158</v>
       </c>
       <c r="B12" s="0">
         <v>16.890000000000001</v>
@@ -2784,10 +2406,19 @@
       <c r="I12" s="0">
         <v>0.071999999999999995</v>
       </c>
+      <c r="J12" s="0">
+        <v>6</v>
+      </c>
+      <c r="K12" s="0">
+        <v>0</v>
+      </c>
+      <c r="L12" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" x14ac:dyDescent="0.45">
       <c r="A13" s="0" t="s">
-        <v>367</v>
+        <v>159</v>
       </c>
       <c r="B13" s="0">
         <v>17.120000000000001</v>
@@ -2813,10 +2444,19 @@
       <c r="I13" s="0">
         <v>0.22500000000000001</v>
       </c>
+      <c r="J13" s="0">
+        <v>10</v>
+      </c>
+      <c r="K13" s="0">
+        <v>0</v>
+      </c>
+      <c r="L13" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" x14ac:dyDescent="0.45">
       <c r="A14" s="0" t="s">
-        <v>368</v>
+        <v>160</v>
       </c>
       <c r="B14" s="0">
         <v>17.490000000000002</v>
@@ -2842,10 +2482,19 @@
       <c r="I14" s="0">
         <v>0.26600000000000001</v>
       </c>
+      <c r="J14" s="0">
+        <v>18</v>
+      </c>
+      <c r="K14" s="0">
+        <v>0</v>
+      </c>
+      <c r="L14" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" x14ac:dyDescent="0.45">
       <c r="A15" s="0" t="s">
-        <v>369</v>
+        <v>161</v>
       </c>
       <c r="B15" s="0">
         <v>18.210000000000001</v>
@@ -2871,10 +2520,19 @@
       <c r="I15" s="0">
         <v>0.091999999999999998</v>
       </c>
+      <c r="J15" s="0">
+        <v>6</v>
+      </c>
+      <c r="K15" s="0">
+        <v>0</v>
+      </c>
+      <c r="L15" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" x14ac:dyDescent="0.45">
       <c r="A16" s="0" t="s">
-        <v>370</v>
+        <v>162</v>
       </c>
       <c r="B16" s="0">
         <v>18.439999999999998</v>
@@ -2900,10 +2558,19 @@
       <c r="I16" s="0">
         <v>0.27000000000000002</v>
       </c>
+      <c r="J16" s="0">
+        <v>18</v>
+      </c>
+      <c r="K16" s="0">
+        <v>0</v>
+      </c>
+      <c r="L16" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" x14ac:dyDescent="0.45">
       <c r="A17" s="0" t="s">
-        <v>371</v>
+        <v>163</v>
       </c>
       <c r="B17" s="0">
         <v>18.84</v>
@@ -2929,10 +2596,19 @@
       <c r="I17" s="0">
         <v>0.058000000000000003</v>
       </c>
+      <c r="J17" s="0">
+        <v>8</v>
+      </c>
+      <c r="K17" s="0">
+        <v>0</v>
+      </c>
+      <c r="L17" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" x14ac:dyDescent="0.45">
       <c r="A18" s="0" t="s">
-        <v>372</v>
+        <v>164</v>
       </c>
       <c r="B18" s="0">
         <v>20.140000000000001</v>
@@ -2958,10 +2634,19 @@
       <c r="I18" s="0">
         <v>0.11</v>
       </c>
+      <c r="J18" s="0">
+        <v>7</v>
+      </c>
+      <c r="K18" s="0">
+        <v>1</v>
+      </c>
+      <c r="L18" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" x14ac:dyDescent="0.45">
       <c r="A19" s="0" t="s">
-        <v>373</v>
+        <v>165</v>
       </c>
       <c r="B19" s="0">
         <v>20.640000000000001</v>
@@ -2987,10 +2672,19 @@
       <c r="I19" s="0">
         <v>0.056000000000000001</v>
       </c>
+      <c r="J19" s="0">
+        <v>8</v>
+      </c>
+      <c r="K19" s="0">
+        <v>0</v>
+      </c>
+      <c r="L19" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" x14ac:dyDescent="0.45">
       <c r="A20" s="0" t="s">
-        <v>374</v>
+        <v>166</v>
       </c>
       <c r="B20" s="0">
         <v>21.120000000000001</v>
@@ -3016,10 +2710,19 @@
       <c r="I20" s="0">
         <v>0.20399999999999999</v>
       </c>
+      <c r="J20" s="0">
+        <v>7</v>
+      </c>
+      <c r="K20" s="0">
+        <v>0</v>
+      </c>
+      <c r="L20" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" x14ac:dyDescent="0.45">
       <c r="A21" s="0" t="s">
-        <v>375</v>
+        <v>167</v>
       </c>
       <c r="B21" s="0">
         <v>21.140000000000001</v>
@@ -3045,10 +2748,19 @@
       <c r="I21" s="0">
         <v>0.46000000000000002</v>
       </c>
+      <c r="J21" s="0">
+        <v>22</v>
+      </c>
+      <c r="K21" s="0">
+        <v>0</v>
+      </c>
+      <c r="L21" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" x14ac:dyDescent="0.45">
       <c r="A22" s="0" t="s">
-        <v>376</v>
+        <v>168</v>
       </c>
       <c r="B22" s="0">
         <v>23.539999999999999</v>
@@ -3074,10 +2786,19 @@
       <c r="I22" s="0">
         <v>0.12</v>
       </c>
+      <c r="J22" s="0">
+        <v>6</v>
+      </c>
+      <c r="K22" s="0">
+        <v>0</v>
+      </c>
+      <c r="L22" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" x14ac:dyDescent="0.45">
       <c r="A23" s="0" t="s">
-        <v>377</v>
+        <v>169</v>
       </c>
       <c r="B23" s="0">
         <v>23.890000000000001</v>
@@ -3103,10 +2824,19 @@
       <c r="I23" s="0">
         <v>0.246</v>
       </c>
+      <c r="J23" s="0">
+        <v>6</v>
+      </c>
+      <c r="K23" s="0">
+        <v>0</v>
+      </c>
+      <c r="L23" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" x14ac:dyDescent="0.45">
       <c r="A24" s="0" t="s">
-        <v>378</v>
+        <v>170</v>
       </c>
       <c r="B24" s="0">
         <v>24.189999999999998</v>
@@ -3131,6 +2861,15 @@
       </c>
       <c r="I24" s="0">
         <v>0.037999999999999999</v>
+      </c>
+      <c r="J24" s="0">
+        <v>9</v>
+      </c>
+      <c r="K24" s="0">
+        <v>0</v>
+      </c>
+      <c r="L24" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3139,12 +2878,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3152,125 +2889,143 @@
     <col min="2" max="2" width="5.64453125" customWidth="true"/>
     <col min="3" max="3" width="11.64453125" customWidth="true"/>
     <col min="5" max="5" width="13.64453125" customWidth="true"/>
-    <col min="6" max="6" width="6.24609375" customWidth="true"/>
-    <col min="7" max="7" width="5.64453125" customWidth="true"/>
-    <col min="8" max="8" width="5.64453125" customWidth="true"/>
-    <col min="9" max="9" width="5.64453125" customWidth="true"/>
-    <col min="10" max="10" width="11.64453125" customWidth="true"/>
-    <col min="11" max="11" width="11.64453125" customWidth="true"/>
-    <col min="12" max="12" width="11.64453125" customWidth="true"/>
+    <col min="6" max="6" width="13.24609375" customWidth="true"/>
+    <col min="7" max="7" width="12.64453125" customWidth="true"/>
+    <col min="8" max="8" width="11.64453125" customWidth="true"/>
+    <col min="9" max="9" width="12.64453125" customWidth="true"/>
+    <col min="10" max="10" width="3.1796875" customWidth="true"/>
+    <col min="11" max="11" width="2.1796875" customWidth="true"/>
+    <col min="12" max="12" width="2.1796875" customWidth="true"/>
+    <col min="20" max="20" width="11.64453125" customWidth="true"/>
+    <col min="21" max="21" width="13.24609375" customWidth="true"/>
+    <col min="4" max="4" width="11.64453125" customWidth="true"/>
     <col min="13" max="13" width="11.64453125" customWidth="true"/>
-    <col min="14" max="14" width="12.64453125" customWidth="true"/>
-    <col min="15" max="15" width="12.64453125" customWidth="true"/>
-    <col min="16" max="16" width="5.64453125" customWidth="true"/>
-    <col min="4" max="4" width="11.64453125" customWidth="true"/>
-    <col min="17" max="17" width="12.64453125" customWidth="true"/>
-    <col min="18" max="18" width="7.24609375" customWidth="true"/>
+    <col min="14" max="14" width="11.64453125" customWidth="true"/>
+    <col min="15" max="15" width="11.64453125" customWidth="true"/>
+    <col min="16" max="16" width="11.64453125" customWidth="true"/>
+    <col min="17" max="17" width="11.64453125" customWidth="true"/>
+    <col min="18" max="18" width="11.64453125" customWidth="true"/>
+    <col min="19" max="19" width="11.64453125" customWidth="true"/>
+    <col min="22" max="22" width="11.64453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.45">
       <c r="A1" s="0" t="s">
-        <v>379</v>
+        <v>171</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>381</v>
+        <v>173</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>382</v>
+        <v>174</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>383</v>
+        <v>175</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>384</v>
+        <v>176</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>385</v>
+        <v>177</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>386</v>
+        <v>178</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>387</v>
+        <v>179</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>388</v>
+        <v>180</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>389</v>
+        <v>181</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>390</v>
+        <v>182</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>391</v>
+        <v>183</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>392</v>
+        <v>184</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>393</v>
+        <v>185</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>394</v>
+        <v>186</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>395</v>
+        <v>187</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>396</v>
+        <v>188</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.45">
       <c r="A2" s="0" t="s">
-        <v>397</v>
+        <v>193</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>398</v>
+        <v>194</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>399</v>
+        <v>195</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>400</v>
+        <v>196</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>400</v>
+        <v>196</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>400</v>
+        <v>196</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>400</v>
+        <v>196</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>400</v>
+        <v>196</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>401</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
       <c r="L2" s="0" t="s">
-        <v>401</v>
+        <v>197</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>401</v>
+        <v>197</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>401</v>
+        <v>197</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.45">
       <c r="A3" s="0" t="s">
-        <v>402</v>
+        <v>198</v>
       </c>
       <c r="B3" s="0">
         <v>12.190000000000001</v>
@@ -3285,10 +3040,10 @@
         <v>0.14363301630762756</v>
       </c>
       <c r="F3" s="0">
-        <v>-2.206</v>
+        <v>-0.87386973604719065</v>
       </c>
       <c r="G3" s="0">
-        <v>0.375</v>
+        <v>1.9703361437657543</v>
       </c>
       <c r="H3" s="0">
         <v>-0.89000000000000001</v>
@@ -3297,36 +3052,48 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="J3" s="0">
-        <v>28.352441634401487</v>
+        <v>10</v>
       </c>
       <c r="K3" s="0">
-        <v>29.30785541095247</v>
+        <v>1</v>
       </c>
       <c r="L3" s="0">
-        <v>29.820540540540541</v>
+        <v>0</v>
       </c>
       <c r="M3" s="0">
-        <v>30.853727076698316</v>
+        <v>22.005233634093749</v>
       </c>
       <c r="N3" s="0">
-        <v>3.7056173370265242</v>
+        <v>17.276464285800646</v>
       </c>
       <c r="O3" s="0">
-        <v>3.8139286534955659</v>
+        <v>22.589655925664509</v>
       </c>
       <c r="P3" s="0">
-        <v>3</v>
+        <v>18.121601463433972</v>
       </c>
       <c r="Q3" s="0">
-        <v>3.7397513513513481</v>
+        <v>24.176091733567489</v>
       </c>
       <c r="R3" s="0">
-        <v>5.9254999999999995</v>
+        <v>14.981297210717196</v>
+      </c>
+      <c r="S3" s="0">
+        <v>24.532156289568011</v>
+      </c>
+      <c r="T3" s="0">
+        <v>17.201516338794018</v>
+      </c>
+      <c r="U3" s="0">
+        <v>-0.42676678917089411</v>
+      </c>
+      <c r="V3" s="0">
+        <v>14.943056814684372</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.45">
       <c r="A4" s="0" t="s">
-        <v>403</v>
+        <v>199</v>
       </c>
       <c r="B4" s="0">
         <v>13.59</v>
@@ -3353,36 +3120,48 @@
         <v>0.81799999999999995</v>
       </c>
       <c r="J4" s="0">
-        <v>21.301445182013083</v>
+        <v>10</v>
       </c>
       <c r="K4" s="0">
-        <v>21.970042230113506</v>
+        <v>0</v>
       </c>
       <c r="L4" s="0">
-        <v>23.90054054054054</v>
+        <v>0</v>
       </c>
       <c r="M4" s="0">
-        <v>23.758703076698318</v>
+        <v>21.317502178539257</v>
       </c>
       <c r="N4" s="0">
-        <v>1.7461243509429778</v>
+        <v>2.7809916505741161</v>
       </c>
       <c r="O4" s="0">
-        <v>1.8369825312791477</v>
+        <v>21.983824012528661</v>
       </c>
       <c r="P4" s="0">
-        <v>1.5199999999999996</v>
+        <v>2.9256994754694481</v>
       </c>
       <c r="Q4" s="0">
-        <v>1.7485833513513498</v>
+        <v>23.905984244997025</v>
       </c>
       <c r="R4" s="0">
-        <v>0.00549999999999784</v>
+        <v>2.4239966118606948</v>
+      </c>
+      <c r="S4" s="0">
+        <v>23.776899609925998</v>
+      </c>
+      <c r="T4" s="0">
+        <v>2.7869385910819973</v>
+      </c>
+      <c r="U4" s="0">
+        <v>-0.69687427774135569</v>
+      </c>
+      <c r="V4" s="0">
+        <v>2.0613792367694694</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.45">
       <c r="A5" s="0" t="s">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="B5" s="0">
         <v>14.59</v>
@@ -3409,36 +3188,48 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="J5" s="0">
-        <v>19.053510283317905</v>
+        <v>6</v>
       </c>
       <c r="K5" s="0">
-        <v>19.596984291686113</v>
+        <v>0</v>
       </c>
       <c r="L5" s="0">
-        <v>21.920540540540543</v>
+        <v>0</v>
       </c>
       <c r="M5" s="0">
-        <v>21.512796434806429</v>
+        <v>19.084993241903597</v>
       </c>
       <c r="N5" s="0">
-        <v>3.878334290039561</v>
+        <v>4.3931166620295681</v>
       </c>
       <c r="O5" s="0">
-        <v>4.1079561303309902</v>
+        <v>19.622589455459376</v>
       </c>
       <c r="P5" s="0">
-        <v>3.4559999999999995</v>
+        <v>4.651926752708361</v>
       </c>
       <c r="Q5" s="0">
-        <v>3.8645295567567572</v>
+        <v>21.92627944233918</v>
       </c>
       <c r="R5" s="0">
-        <v>-1.974499999999999</v>
+        <v>3.9136931571464615</v>
+      </c>
+      <c r="S5" s="0">
+        <v>21.550323525862435</v>
+      </c>
+      <c r="T5" s="0">
+        <v>4.3775248484982754</v>
+      </c>
+      <c r="U5" s="0">
+        <v>-2.676579080399196</v>
+      </c>
+      <c r="V5" s="0">
+        <v>3.7156797204096192</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.45">
       <c r="A6" s="0" t="s">
-        <v>405</v>
+        <v>201</v>
       </c>
       <c r="B6" s="0">
         <v>15.02</v>
@@ -3452,23 +3243,61 @@
       <c r="E6" s="0">
         <v>0.10350965730875188</v>
       </c>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
-      <c r="J6" s="0"/>
-      <c r="K6" s="0"/>
-      <c r="L6" s="0"/>
-      <c r="M6" s="0"/>
-      <c r="N6" s="0"/>
-      <c r="O6" s="0"/>
-      <c r="P6" s="0"/>
-      <c r="Q6" s="0"/>
-      <c r="R6" s="0"/>
+      <c r="F6" s="0">
+        <v>-0.15657041491121942</v>
+      </c>
+      <c r="G6" s="0">
+        <v>0.15658315377321824</v>
+      </c>
+      <c r="H6" s="0">
+        <v>4.4725361218805384</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0.10379699156144404</v>
+      </c>
+      <c r="J6" s="0">
+        <v>12</v>
+      </c>
+      <c r="K6" s="0">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0">
+        <v>18.734460692615674</v>
+      </c>
+      <c r="N6" s="0">
+        <v>2.509366656250219</v>
+      </c>
+      <c r="O6" s="0">
+        <v>19.256335670411335</v>
+      </c>
+      <c r="P6" s="0">
+        <v>2.6606103874302351</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>21.628551751247773</v>
+      </c>
+      <c r="R6" s="0">
+        <v>2.2461490883574551</v>
+      </c>
+      <c r="S6" s="0">
+        <v>21.197231731363967</v>
+      </c>
+      <c r="T6" s="0">
+        <v>2.4998635351164071</v>
+      </c>
+      <c r="U6" s="0">
+        <v>-2.9743067714906091</v>
+      </c>
+      <c r="V6" s="0">
+        <v>1.87261848519567</v>
+      </c>
     </row>
     <row r="7" x14ac:dyDescent="0.45">
       <c r="A7" s="0" t="s">
-        <v>406</v>
+        <v>202</v>
       </c>
       <c r="B7" s="0">
         <v>15.289999999999999</v>
@@ -3495,36 +3324,48 @@
         <v>0.23999999999999999</v>
       </c>
       <c r="J7" s="0">
-        <v>19.878424297902825</v>
+        <v>15</v>
       </c>
       <c r="K7" s="0">
-        <v>20.469700284013811</v>
+        <v>0</v>
       </c>
       <c r="L7" s="0">
-        <v>22.652540540540542</v>
+        <v>0</v>
       </c>
       <c r="M7" s="0">
-        <v>22.335678834536157</v>
+        <v>19.902199067709432</v>
       </c>
       <c r="N7" s="0">
-        <v>2.9338475410010574</v>
+        <v>3.630761811576575</v>
       </c>
       <c r="O7" s="0">
-        <v>3.0998610144577015</v>
+        <v>20.4895266657349</v>
       </c>
       <c r="P7" s="0">
-        <v>2.5919999999999987</v>
+        <v>3.8353045006379127</v>
       </c>
       <c r="Q7" s="0">
-        <v>2.9292290075675638</v>
+        <v>22.658553167757486</v>
       </c>
       <c r="R7" s="0">
-        <v>-1.2424999999999997</v>
+        <v>3.2076247143300969</v>
+      </c>
+      <c r="S7" s="0">
+        <v>22.363371170488609</v>
+      </c>
+      <c r="T7" s="0">
+        <v>3.6261946798206215</v>
+      </c>
+      <c r="U7" s="0">
+        <v>-1.9443053549808882</v>
+      </c>
+      <c r="V7" s="0">
+        <v>2.9431693322535106</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.45">
       <c r="A8" s="0" t="s">
-        <v>407</v>
+        <v>203</v>
       </c>
       <c r="B8" s="0">
         <v>15.640000000000001</v>
@@ -3551,36 +3392,48 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="J8" s="0">
-        <v>17.942432396368304</v>
+        <v>6</v>
       </c>
       <c r="K8" s="0">
-        <v>18.418070260754973</v>
+        <v>0</v>
       </c>
       <c r="L8" s="0">
-        <v>20.924540540540541</v>
+        <v>0</v>
       </c>
       <c r="M8" s="0">
-        <v>20.40712061615778</v>
+        <v>17.967717384565571</v>
       </c>
       <c r="N8" s="0">
-        <v>3.2209299331026386</v>
+        <v>3.8351595906003486</v>
       </c>
       <c r="O8" s="0">
-        <v>3.4231724473782492</v>
+        <v>18.439051005584229</v>
       </c>
       <c r="P8" s="0">
-        <v>2.9039999999999964</v>
+        <v>4.0750163394671519</v>
       </c>
       <c r="Q8" s="0">
-        <v>3.2002770681081074</v>
+        <v>20.930110078889523</v>
       </c>
       <c r="R8" s="0">
-        <v>-2.9705000000000013</v>
+        <v>3.4572390727576452</v>
+      </c>
+      <c r="S8" s="0">
+        <v>20.437534723766721</v>
+      </c>
+      <c r="T8" s="0">
+        <v>3.8108179362415835</v>
+      </c>
+      <c r="U8" s="0">
+        <v>-3.6727484438488545</v>
+      </c>
+      <c r="V8" s="0">
+        <v>3.2141612377218727</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.45">
       <c r="A9" s="0" t="s">
-        <v>408</v>
+        <v>204</v>
       </c>
       <c r="B9" s="0">
         <v>15.940000000000001</v>
@@ -3607,36 +3460,48 @@
         <v>0.108</v>
       </c>
       <c r="J9" s="0">
-        <v>21.434791457803613</v>
+        <v>6</v>
       </c>
       <c r="K9" s="0">
-        <v>22.110300220951274</v>
+        <v>0</v>
       </c>
       <c r="L9" s="0">
-        <v>24.016540540540539</v>
+        <v>0</v>
       </c>
       <c r="M9" s="0">
-        <v>23.892256925617239</v>
+        <v>21.460475267013734</v>
       </c>
       <c r="N9" s="0">
-        <v>3.2672110482305357</v>
+        <v>3.9106184049378729</v>
       </c>
       <c r="O9" s="0">
-        <v>3.4357079118312868</v>
+        <v>22.131157294962257</v>
       </c>
       <c r="P9" s="0">
-        <v>2.8399999999999999</v>
+        <v>4.1123914574144891</v>
       </c>
       <c r="Q9" s="0">
-        <v>3.2724433459459448</v>
+        <v>24.021802776272271</v>
       </c>
       <c r="R9" s="0">
-        <v>0.1214999999999975</v>
+        <v>3.4025448880682592</v>
+      </c>
+      <c r="S9" s="0">
+        <v>23.921834723354525</v>
+      </c>
+      <c r="T9" s="0">
+        <v>3.9172831064751383</v>
+      </c>
+      <c r="U9" s="0">
+        <v>-0.58105574646610481</v>
+      </c>
+      <c r="V9" s="0">
+        <v>3.1765953647655012</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.45">
       <c r="A10" s="0" t="s">
-        <v>409</v>
+        <v>205</v>
       </c>
       <c r="B10" s="0">
         <v>16.190000000000001</v>
@@ -3663,36 +3528,48 @@
         <v>0.249</v>
       </c>
       <c r="J10" s="0">
-        <v>22.443146441717374</v>
+        <v>5</v>
       </c>
       <c r="K10" s="0">
-        <v>23.169067921177884</v>
+        <v>0</v>
       </c>
       <c r="L10" s="0">
-        <v>24.888540540540539</v>
+        <v>0</v>
       </c>
       <c r="M10" s="0">
-        <v>24.903213425076697</v>
+        <v>22.46265725325545</v>
       </c>
       <c r="N10" s="0">
-        <v>2.4179829599808045</v>
+        <v>3.2430225672978699</v>
       </c>
       <c r="O10" s="0">
-        <v>2.534882856019351</v>
+        <v>23.185286936764648</v>
       </c>
       <c r="P10" s="0">
-        <v>2.0800000000000018</v>
+        <v>3.3994964514809811</v>
       </c>
       <c r="Q10" s="0">
-        <v>2.4261926702702716</v>
+        <v>24.893828213021123</v>
       </c>
       <c r="R10" s="0">
-        <v>0.99349999999999739</v>
+        <v>2.7920757129274341</v>
+      </c>
+      <c r="S10" s="0">
+        <v>24.925214803791405</v>
+      </c>
+      <c r="T10" s="0">
+        <v>3.2560504123512457</v>
+      </c>
+      <c r="U10" s="0">
+        <v>0.29096969028273439</v>
+      </c>
+      <c r="V10" s="0">
+        <v>2.4915235088832546</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.45">
       <c r="A11" s="0" t="s">
-        <v>410</v>
+        <v>206</v>
       </c>
       <c r="B11" s="0">
         <v>16.539999999999999</v>
@@ -3719,36 +3596,48 @@
         <v>0.084000000000000005</v>
       </c>
       <c r="J11" s="0">
-        <v>20.314030362224571</v>
+        <v>6</v>
       </c>
       <c r="K11" s="0">
-        <v>20.929666836847957</v>
+        <v>0</v>
       </c>
       <c r="L11" s="0">
-        <v>23.036540540540543</v>
+        <v>0</v>
       </c>
       <c r="M11" s="0">
-        <v>22.770836767509127</v>
+        <v>20.332341345972022</v>
       </c>
       <c r="N11" s="0">
-        <v>2.2467504372580152</v>
+        <v>3.0743252765283193</v>
       </c>
       <c r="O11" s="0">
-        <v>2.3707738511602656</v>
+        <v>20.945191214316161</v>
       </c>
       <c r="P11" s="0">
-        <v>1.9759999999999991</v>
+        <v>3.2436515837489202</v>
       </c>
       <c r="Q11" s="0">
-        <v>2.2454153167567554</v>
+        <v>23.042015586278627</v>
       </c>
       <c r="R11" s="0">
-        <v>-0.85849999999999937</v>
+        <v>2.7054481876661542</v>
+      </c>
+      <c r="S11" s="0">
+        <v>22.791924691093858</v>
+      </c>
+      <c r="T11" s="0">
+        <v>3.0739498093389499</v>
+      </c>
+      <c r="U11" s="0">
+        <v>-1.560842936459742</v>
+      </c>
+      <c r="V11" s="0">
+        <v>2.4128766033965157</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.45">
       <c r="A12" s="0" t="s">
-        <v>411</v>
+        <v>207</v>
       </c>
       <c r="B12" s="0">
         <v>16.890000000000001</v>
@@ -3775,36 +3664,48 @@
         <v>0.071999999999999995</v>
       </c>
       <c r="J12" s="0">
-        <v>20.186773638013847</v>
+        <v>6</v>
       </c>
       <c r="K12" s="0">
-        <v>20.795356562389486</v>
+        <v>0</v>
       </c>
       <c r="L12" s="0">
-        <v>22.924540540540541</v>
+        <v>0</v>
       </c>
       <c r="M12" s="0">
-        <v>22.643668183725346</v>
+        <v>20.202782299882386</v>
       </c>
       <c r="N12" s="0">
-        <v>1.5805983335544624</v>
+        <v>2.6259666188544601</v>
       </c>
       <c r="O12" s="0">
-        <v>1.6685133642878895</v>
+        <v>20.809485253028484</v>
       </c>
       <c r="P12" s="0">
-        <v>1.3919999999999959</v>
+        <v>2.7713532252975441</v>
       </c>
       <c r="Q12" s="0">
-        <v>1.5792571070270256</v>
+        <v>22.930933296049364</v>
       </c>
       <c r="R12" s="0">
-        <v>-0.97050000000000125</v>
+        <v>2.3134338348531061</v>
+      </c>
+      <c r="S12" s="0">
+        <v>22.661791363290767</v>
+      </c>
+      <c r="T12" s="0">
+        <v>2.6260588485805876</v>
+      </c>
+      <c r="U12" s="0">
+        <v>-1.6719252266890108</v>
+      </c>
+      <c r="V12" s="0">
+        <v>1.953448869563531</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.45">
       <c r="A13" s="0" t="s">
-        <v>412</v>
+        <v>208</v>
       </c>
       <c r="B13" s="0">
         <v>17.120000000000001</v>
@@ -3831,36 +3732,48 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="J13" s="0">
-        <v>20.687686274983093</v>
+        <v>10</v>
       </c>
       <c r="K13" s="0">
-        <v>21.32373279008857</v>
+        <v>0</v>
       </c>
       <c r="L13" s="0">
-        <v>23.364540540540538</v>
+        <v>0</v>
       </c>
       <c r="M13" s="0">
-        <v>23.144431648590214</v>
+        <v>20.71127962485355</v>
       </c>
       <c r="N13" s="0">
-        <v>3.0044170490835427</v>
+        <v>3.690519936325205</v>
       </c>
       <c r="O13" s="0">
-        <v>3.166603401854843</v>
+        <v>21.343125548759318</v>
       </c>
       <c r="P13" s="0">
-        <v>2.6320000000000014</v>
+        <v>3.8892049886738982</v>
       </c>
       <c r="Q13" s="0">
-        <v>3.004885398918919</v>
+        <v>23.369882841077594</v>
       </c>
       <c r="R13" s="0">
-        <v>-0.53050000000000352</v>
+        <v>3.2344132129606091</v>
+      </c>
+      <c r="S13" s="0">
+        <v>23.171778697284967</v>
+      </c>
+      <c r="T13" s="0">
+        <v>3.6919066450829234</v>
+      </c>
+      <c r="U13" s="0">
+        <v>-1.2329756816608139</v>
+      </c>
+      <c r="V13" s="0">
+        <v>2.9580383801312928</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.45">
       <c r="A14" s="0" t="s">
-        <v>413</v>
+        <v>209</v>
       </c>
       <c r="B14" s="0">
         <v>17.490000000000002</v>
@@ -3887,36 +3800,48 @@
         <v>0.26600000000000001</v>
       </c>
       <c r="J14" s="0">
-        <v>22.578083932797654</v>
+        <v>18</v>
       </c>
       <c r="K14" s="0">
-        <v>23.310503169036622</v>
+        <v>0</v>
       </c>
       <c r="L14" s="0">
-        <v>25.004540540540539</v>
+        <v>0</v>
       </c>
       <c r="M14" s="0">
-        <v>25.038629653995617</v>
+        <v>22.59583659803209</v>
       </c>
       <c r="N14" s="0">
-        <v>2.1512711636484028</v>
+        <v>3.0237923292946132</v>
       </c>
       <c r="O14" s="0">
-        <v>2.2543526140847803</v>
+        <v>23.325424191620975</v>
       </c>
       <c r="P14" s="0">
-        <v>1.8480000000000025</v>
+        <v>3.1687181444837949</v>
       </c>
       <c r="Q14" s="0">
-        <v>2.1590623524324357</v>
+        <v>25.009837573665216</v>
       </c>
       <c r="R14" s="0">
-        <v>1.109499999999997</v>
+        <v>2.6009576933778757</v>
+      </c>
+      <c r="S14" s="0">
+        <v>25.058558525116986</v>
+      </c>
+      <c r="T14" s="0">
+        <v>3.0368576001388687</v>
+      </c>
+      <c r="U14" s="0">
+        <v>0.40697905092680042</v>
+      </c>
+      <c r="V14" s="0">
+        <v>2.3121791223159467</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.45">
       <c r="A15" s="0" t="s">
-        <v>414</v>
+        <v>210</v>
       </c>
       <c r="B15" s="0">
         <v>18.210000000000001</v>
@@ -3943,36 +3868,48 @@
         <v>0.091999999999999998</v>
       </c>
       <c r="J15" s="0">
-        <v>24.126991680942297</v>
+        <v>6</v>
       </c>
       <c r="K15" s="0">
-        <v>24.929792963240232</v>
+        <v>0</v>
       </c>
       <c r="L15" s="0">
-        <v>26.324540540540539</v>
+        <v>0</v>
       </c>
       <c r="M15" s="0">
-        <v>26.594974048590213</v>
+        <v>24.213858019510472</v>
       </c>
       <c r="N15" s="0">
-        <v>7.7060460653088967</v>
+        <v>7.9766298252898995</v>
       </c>
       <c r="O15" s="0">
-        <v>8.0350061567987154</v>
+        <v>24.994719235158001</v>
       </c>
       <c r="P15" s="0">
-        <v>6.5120000000000005</v>
+        <v>8.3106875110396921</v>
       </c>
       <c r="Q15" s="0">
-        <v>7.7478068799999953</v>
+        <v>26.329057003491627</v>
       </c>
       <c r="R15" s="0">
-        <v>2.4294999999999973</v>
+        <v>6.7321154529925522</v>
+      </c>
+      <c r="S15" s="0">
+        <v>26.692397627659258</v>
+      </c>
+      <c r="T15" s="0">
+        <v>8.0142552222143095</v>
+      </c>
+      <c r="U15" s="0">
+        <v>1.7261984807532549</v>
+      </c>
+      <c r="V15" s="0">
+        <v>6.6695720079224783</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.45">
       <c r="A16" s="0" t="s">
-        <v>415</v>
+        <v>211</v>
       </c>
       <c r="B16" s="0">
         <v>18.439999999999998</v>
@@ -3999,36 +3936,48 @@
         <v>0.27000000000000002</v>
       </c>
       <c r="J16" s="0">
-        <v>26.584966056638564</v>
+        <v>18</v>
       </c>
       <c r="K16" s="0">
-        <v>27.483563905581775</v>
+        <v>0</v>
       </c>
       <c r="L16" s="0">
-        <v>28.376540540540539</v>
+        <v>1</v>
       </c>
       <c r="M16" s="0">
-        <v>29.070601822914533</v>
+        <v>26.613994570771879</v>
       </c>
       <c r="N16" s="0">
-        <v>3.5618468442275457</v>
+        <v>4.2015966167143102</v>
       </c>
       <c r="O16" s="0">
-        <v>3.6863321663659008</v>
+        <v>27.506474557605269</v>
       </c>
       <c r="P16" s="0">
-        <v>2.9359999999999964</v>
+        <v>4.3472380856980388</v>
       </c>
       <c r="Q16" s="0">
-        <v>3.5910767491891846</v>
+        <v>28.382128655045182</v>
       </c>
       <c r="R16" s="0">
-        <v>4.4814999999999969</v>
+        <v>3.4641532291841046</v>
+      </c>
+      <c r="S16" s="0">
+        <v>29.101810293243428</v>
+      </c>
+      <c r="T16" s="0">
+        <v>4.238440977194494</v>
+      </c>
+      <c r="U16" s="0">
+        <v>3.7792701323068214</v>
+      </c>
+      <c r="V16" s="0">
+        <v>3.2320147486780906</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.45">
       <c r="A17" s="0" t="s">
-        <v>416</v>
+        <v>212</v>
       </c>
       <c r="B17" s="0">
         <v>18.84</v>
@@ -4055,36 +4004,48 @@
         <v>0.058000000000000003</v>
       </c>
       <c r="J17" s="0">
-        <v>21.117822400884393</v>
+        <v>8</v>
       </c>
       <c r="K17" s="0">
-        <v>21.776808113303218</v>
+        <v>0</v>
       </c>
       <c r="L17" s="0">
-        <v>23.740540540540543</v>
+        <v>0</v>
       </c>
       <c r="M17" s="0">
-        <v>23.574849671292917</v>
+        <v>21.130578739189065</v>
       </c>
       <c r="N17" s="0">
-        <v>0.35772273790041709</v>
+        <v>2.1360191297162481</v>
       </c>
       <c r="O17" s="0">
-        <v>0.37655243486779</v>
+        <v>21.788400935273778</v>
       </c>
       <c r="P17" s="0">
-        <v>0.31200000000000117</v>
+        <v>2.2484659154608582</v>
       </c>
       <c r="Q17" s="0">
-        <v>0.35810854054054175</v>
+        <v>23.746707579546403</v>
       </c>
       <c r="R17" s="0">
-        <v>-0.15449999999999875</v>
+        <v>1.8663590899848561</v>
+      </c>
+      <c r="S17" s="0">
+        <v>23.58900314563973</v>
+      </c>
+      <c r="T17" s="0">
+        <v>2.1416330977372091</v>
+      </c>
+      <c r="U17" s="0">
+        <v>-0.85615094319196194</v>
+      </c>
+      <c r="V17" s="0">
+        <v>1.3751133428049778</v>
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.45">
       <c r="A18" s="0" t="s">
-        <v>417</v>
+        <v>213</v>
       </c>
       <c r="B18" s="0">
         <v>20.140000000000001</v>
@@ -4099,10 +4060,10 @@
         <v>0.11800414700884421</v>
       </c>
       <c r="F18" s="0">
-        <v>-2.867</v>
+        <v>-1.2753413669697196</v>
       </c>
       <c r="G18" s="0">
-        <v>0.32100000000000001</v>
+        <v>0.58535127587614288</v>
       </c>
       <c r="H18" s="0">
         <v>1.5680000000000001</v>
@@ -4111,36 +4072,48 @@
         <v>0.11</v>
       </c>
       <c r="J18" s="0">
-        <v>31.673154316751209</v>
+        <v>7</v>
       </c>
       <c r="K18" s="0">
-        <v>32.707967777469037</v>
+        <v>1</v>
       </c>
       <c r="L18" s="0">
-        <v>32.46454054054054</v>
+        <v>0</v>
       </c>
       <c r="M18" s="0">
-        <v>34.206494331022647</v>
+        <v>23.910360987649668</v>
       </c>
       <c r="N18" s="0">
-        <v>3.280073223415684</v>
+        <v>5.9318410390106946</v>
       </c>
       <c r="O18" s="0">
-        <v>3.3407148417139751</v>
+        <v>24.68959726703018</v>
       </c>
       <c r="P18" s="0">
-        <v>2.5680000000000049</v>
+        <v>6.1883878134994434</v>
       </c>
       <c r="Q18" s="0">
-        <v>3.3115612767567626</v>
+        <v>26.103013473134411</v>
       </c>
       <c r="R18" s="0">
-        <v>8.5694999999999979</v>
+        <v>5.0256028679536442</v>
+      </c>
+      <c r="S18" s="0">
+        <v>26.383103189094491</v>
+      </c>
+      <c r="T18" s="0">
+        <v>5.9620077670621816</v>
+      </c>
+      <c r="U18" s="0">
+        <v>1.5001549503960379</v>
+      </c>
+      <c r="V18" s="0">
+        <v>4.8567847941222295</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.45">
       <c r="A19" s="0" t="s">
-        <v>418</v>
+        <v>214</v>
       </c>
       <c r="B19" s="0">
         <v>20.640000000000001</v>
@@ -4167,36 +4140,48 @@
         <v>0.056000000000000001</v>
       </c>
       <c r="J19" s="0">
-        <v>25.341044758237672</v>
+        <v>8</v>
       </c>
       <c r="K19" s="0">
-        <v>26.193601118151435</v>
+        <v>0</v>
       </c>
       <c r="L19" s="0">
-        <v>27.344540540540542</v>
+        <v>0</v>
       </c>
       <c r="M19" s="0">
-        <v>27.81699655804967</v>
+        <v>25.356341934856083</v>
       </c>
       <c r="N19" s="0">
-        <v>1.5426672504523822</v>
+        <v>2.698339150258493</v>
       </c>
       <c r="O19" s="0">
-        <v>1.60285060882984</v>
+        <v>26.206555764844843</v>
       </c>
       <c r="P19" s="0">
-        <v>1.2880000000000003</v>
+        <v>2.8040084202988482</v>
       </c>
       <c r="Q19" s="0">
-        <v>1.5537772335135145</v>
+        <v>27.349737800697532</v>
       </c>
       <c r="R19" s="0">
-        <v>3.4495000000000005</v>
+        <v>2.2584279332322548</v>
+      </c>
+      <c r="S19" s="0">
+        <v>27.833625833931215</v>
+      </c>
+      <c r="T19" s="0">
+        <v>2.7216827251651807</v>
+      </c>
+      <c r="U19" s="0">
+        <v>2.746879277959152</v>
+      </c>
+      <c r="V19" s="0">
+        <v>1.8996070081936693</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.45">
       <c r="A20" s="0" t="s">
-        <v>419</v>
+        <v>215</v>
       </c>
       <c r="B20" s="0">
         <v>21.120000000000001</v>
@@ -4223,36 +4208,48 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="J20" s="0">
-        <v>21.241729272453995</v>
+        <v>7</v>
       </c>
       <c r="K20" s="0">
-        <v>21.907212525319437</v>
+        <v>0</v>
       </c>
       <c r="L20" s="0">
-        <v>23.84854054054054</v>
+        <v>0</v>
       </c>
       <c r="M20" s="0">
-        <v>23.698905089941562</v>
+        <v>21.265651515627557</v>
       </c>
       <c r="N20" s="0">
-        <v>3.0493697293505306</v>
+        <v>3.7279576380428234</v>
       </c>
       <c r="O20" s="0">
-        <v>3.2085446769575015</v>
+        <v>21.926794224353639</v>
       </c>
       <c r="P20" s="0">
-        <v>2.6559999999999988</v>
+        <v>3.9219303410960058</v>
       </c>
       <c r="Q20" s="0">
-        <v>3.0531750097297277</v>
+        <v>23.853856221639273</v>
       </c>
       <c r="R20" s="0">
-        <v>-0.046500000000001762</v>
+        <v>3.2482247932891051</v>
+      </c>
+      <c r="S20" s="0">
+        <v>23.726445404195967</v>
+      </c>
+      <c r="T20" s="0">
+        <v>3.7336896581596384</v>
+      </c>
+      <c r="U20" s="0">
+        <v>-0.74900230109914667</v>
+      </c>
+      <c r="V20" s="0">
+        <v>2.9737510231919453</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.45">
       <c r="A21" s="0" t="s">
-        <v>420</v>
+        <v>216</v>
       </c>
       <c r="B21" s="0">
         <v>21.140000000000001</v>
@@ -4279,36 +4276,48 @@
         <v>0.46000000000000002</v>
       </c>
       <c r="J21" s="0">
-        <v>25.22134806813915</v>
+        <v>22</v>
       </c>
       <c r="K21" s="0">
-        <v>26.069210411302436</v>
+        <v>0</v>
       </c>
       <c r="L21" s="0">
-        <v>27.244540540540541</v>
+        <v>0</v>
       </c>
       <c r="M21" s="0">
-        <v>27.696442929671292</v>
+        <v>25.281483602854049</v>
       </c>
       <c r="N21" s="0">
-        <v>6.174271675177863</v>
+        <v>6.5405046642391138</v>
       </c>
       <c r="O21" s="0">
-        <v>6.4165957937539133</v>
+        <v>26.114443920648796</v>
       </c>
       <c r="P21" s="0">
-        <v>5.1599999999999966</v>
+        <v>6.7940587466742137</v>
       </c>
       <c r="Q21" s="0">
-        <v>6.2163747243243215</v>
+        <v>27.249206007760357</v>
       </c>
       <c r="R21" s="0">
-        <v>3.349499999999999</v>
+        <v>5.4636064012880556</v>
+      </c>
+      <c r="S21" s="0">
+        <v>27.762692475770901</v>
+      </c>
+      <c r="T21" s="0">
+        <v>6.5827689115554264</v>
+      </c>
+      <c r="U21" s="0">
+        <v>2.6463474850219804</v>
+      </c>
+      <c r="V21" s="0">
+        <v>5.341795975271741</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.45">
       <c r="A22" s="0" t="s">
-        <v>421</v>
+        <v>217</v>
       </c>
       <c r="B22" s="0">
         <v>23.539999999999999</v>
@@ -4335,36 +4344,48 @@
         <v>0.12</v>
       </c>
       <c r="J22" s="0">
-        <v>22.619999471564427</v>
+        <v>6</v>
       </c>
       <c r="K22" s="0">
-        <v>23.354425158926517</v>
+        <v>0</v>
       </c>
       <c r="L22" s="0">
-        <v>25.04054054054054</v>
+        <v>0</v>
       </c>
       <c r="M22" s="0">
-        <v>25.080699840211832</v>
+        <v>22.638046262102524</v>
       </c>
       <c r="N22" s="0">
-        <v>2.1335703896642713</v>
+        <v>3.0599061394159333</v>
       </c>
       <c r="O22" s="0">
-        <v>2.2355162191215072</v>
+        <v>23.369563474288309</v>
       </c>
       <c r="P22" s="0">
-        <v>1.8320000000000007</v>
+        <v>3.2066082909846401</v>
       </c>
       <c r="Q22" s="0">
-        <v>2.1414408918918895</v>
+        <v>25.045847320147221</v>
       </c>
       <c r="R22" s="0">
-        <v>1.1454999999999984</v>
+        <v>2.6323109710638541</v>
+      </c>
+      <c r="S22" s="0">
+        <v>25.100976458112214</v>
+      </c>
+      <c r="T22" s="0">
+        <v>3.072903105937439</v>
+      </c>
+      <c r="U22" s="0">
+        <v>0.44298879740884667</v>
+      </c>
+      <c r="V22" s="0">
+        <v>2.2877083789690289</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.45">
       <c r="A23" s="0" t="s">
-        <v>422</v>
+        <v>218</v>
       </c>
       <c r="B23" s="0">
         <v>23.890000000000001</v>
@@ -4391,36 +4412,48 @@
         <v>0.246</v>
       </c>
       <c r="J23" s="0">
-        <v>25.345835685050019</v>
+        <v>6</v>
       </c>
       <c r="K23" s="0">
-        <v>26.198578962472311</v>
+        <v>0</v>
       </c>
       <c r="L23" s="0">
-        <v>27.34854054054054</v>
+        <v>0</v>
       </c>
       <c r="M23" s="0">
-        <v>27.821822083184806</v>
+        <v>25.360783861425148</v>
       </c>
       <c r="N23" s="0">
-        <v>1.3702574748288612</v>
+        <v>2.6150774628510693</v>
       </c>
       <c r="O23" s="0">
-        <v>1.4236964080063217</v>
+        <v>26.211349295805277</v>
       </c>
       <c r="P23" s="0">
-        <v>1.1440000000000019</v>
+        <v>2.7172176818459097</v>
       </c>
       <c r="Q23" s="0">
-        <v>1.3801373686486542</v>
+        <v>27.353923814968677</v>
       </c>
       <c r="R23" s="0">
-        <v>3.4534999999999982</v>
+        <v>2.1882269338796898</v>
+      </c>
+      <c r="S23" s="0">
+        <v>27.838042112248541</v>
+      </c>
+      <c r="T23" s="0">
+        <v>2.6382050357455227</v>
+      </c>
+      <c r="U23" s="0">
+        <v>2.7510652922303191</v>
+      </c>
+      <c r="V23" s="0">
+        <v>1.7705814200975467</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.45">
       <c r="A24" s="0" t="s">
-        <v>423</v>
+        <v>219</v>
       </c>
       <c r="B24" s="0">
         <v>24.189999999999998</v>
@@ -4447,31 +4480,43 @@
         <v>0.037999999999999999</v>
       </c>
       <c r="J24" s="0">
-        <v>22.104309481771111</v>
+        <v>9</v>
       </c>
       <c r="K24" s="0">
-        <v>22.81365608236473</v>
+        <v>0</v>
       </c>
       <c r="L24" s="0">
-        <v>24.596540540540541</v>
+        <v>0</v>
       </c>
       <c r="M24" s="0">
-        <v>24.563306070211834</v>
+        <v>22.120429547036395</v>
       </c>
       <c r="N24" s="0">
-        <v>1.5383341688890368</v>
+        <v>2.6430989834287084</v>
       </c>
       <c r="O24" s="0">
-        <v>1.6144086027890125</v>
+        <v>22.827760947671347</v>
       </c>
       <c r="P24" s="0">
-        <v>1.3279999999999994</v>
+        <v>2.7736609024548549</v>
       </c>
       <c r="Q24" s="0">
-        <v>1.5427293448648634</v>
+        <v>24.602858522738401</v>
       </c>
       <c r="R24" s="0">
-        <v>0.70149999999999935</v>
+        <v>2.2845726697901756</v>
+      </c>
+      <c r="S24" s="0">
+        <v>24.581246541843221</v>
+      </c>
+      <c r="T24" s="0">
+        <v>2.6535411587089919</v>
+      </c>
+      <c r="U24" s="0">
+        <v>0</v>
+      </c>
+      <c r="V24" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4480,21 +4525,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A0F56654C37D7A4AAC59B6C288F9CE16" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="563f837eafd1d134d0191c976a557f73">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7fa73a2b-a877-44bc-b864-c31a95c8f621" xmlns:ns4="4bb6f66d-1447-4ffa-a850-4f1b35540af2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f764ae2895bc9eb9b73becb11c151bc" ns3:_="" ns4:_="">
     <xsd:import namespace="7fa73a2b-a877-44bc-b864-c31a95c8f621"/>
@@ -4717,24 +4747,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45DDE364-39F5-4CB5-B004-A75D4718A354}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B0DCBC-551C-4D59-922B-DAF738475938}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F8399FD-C108-4E5D-8E4F-378098980073}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4751,4 +4779,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45DDE364-39F5-4CB5-B004-A75D4718A354}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B0DCBC-551C-4D59-922B-DAF738475938}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>